<commit_message>
FMEA fertig, Dokumentation weiter und CE-Beurteilung so gut wei abgeschlossen
</commit_message>
<xml_diff>
--- a/RB-Blessing/CE-Beurteilung.xlsx
+++ b/RB-Blessing/CE-Beurteilung.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20340"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thofmann\Documents\GitHub\KE3\RB-Blessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\langohra.tmb18\Documents\GitHub\KE3\RB-Blessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC76F1D-48D5-4E47-9063-873D105FF460}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="806"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="806" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grenzen der Maschine" sheetId="1" r:id="rId1"/>
@@ -39,7 +40,7 @@
     <definedName name="Liste11">#REF!</definedName>
     <definedName name="Ursprung">'Ursprung-Folgen nach ISO 12100'!$C$11:$C$108</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="455">
   <si>
     <t>Betriebsarten:</t>
   </si>
@@ -1855,9 +1856,6 @@
     <t>Verwendungstemperaturen: -10°C bis 40°C</t>
   </si>
   <si>
-    <t>Durch die stufenlose Regelung der Geschwindigkeit und dem damit verbundenen leistungsstarken Elektromotor kann das Förderband individuell in Betrieb genommen werden.</t>
-  </si>
-  <si>
     <t>Mit einer Bandbreite von 240 mm kann eine Vielzahl von Gütern transportiert werden.</t>
   </si>
   <si>
@@ -1867,55 +1865,73 @@
     <t xml:space="preserve">Die Höhe der Antriebstrommel über dem Boden beläuft sich auf mindestens 300mm bzgl. des Untertrums. </t>
   </si>
   <si>
-    <t>Die Lebensdauer beträgt 30000h.</t>
-  </si>
-  <si>
-    <t>Steigung bis zu 10%</t>
-  </si>
-  <si>
-    <t>Der Bandförderer kann sowohl in einer Halle als auch draußen genutzt werden.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Für den Elektromotor sollte sich ein ein Netzanschluss in nächster Nähe befinden. </t>
   </si>
   <si>
     <t xml:space="preserve">Auch Mitarbeiter des Lagers und der Logistik können die Produkte beim Transport beschädigen. </t>
   </si>
   <si>
-    <t>Ebenso der Transport zum Kunde stellt ein hohes Risiko für Transportschäden dar. Das Produkt kann unter Umständen nicht fristgerecht geliefert werden oder Bestandteile davon fehlen.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bei der Inbetriebnahme des Bandförderers kann die Montageanleitung nicht ausreichend genau gelesen werden und dadurch das Produkt fehlerhaft zusammengebaut werden. </t>
   </si>
   <si>
-    <t xml:space="preserve">Während der ersten Lebensphase, der Produktion / Montage des Bandförderers, sind Mitarbeiter der Fertigung und Montage in direktem Kontakt mit dem Produkt. Eigenangefertige Teile können fehlerhaft produziert werden. Zukaufteile können ebenso fehlerhaft produziert oder beim Transport beschädigt worden sein. </t>
-  </si>
-  <si>
-    <t>Der Bandförderer dient dem Transport von leichten bis mittelschweren Gütern auf waagerechtem oder leicht steigendem Untergrund. Die Güter werden auf das sich bewegende Band gelegt und vom Bandanfang bis Bandende transportiert. Das Band wird von einer Antriebsrolle angetrieben, das widerrum von einem Elektromotor angetrieben wird.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Der Kunde kann beim Einrichten des Produktes durch einen falschen Netzanschluss den Elektromotor beschädigen. </t>
   </si>
   <si>
     <t xml:space="preserve">Tritt ein Fehlerfall ein, bei dem ein Austausch von Teilen notwendig ist, ist darauf zu achten, dass Ersatzteile verwendet werden, die den Vorgaben des Herstellers entsprechen. </t>
   </si>
   <si>
-    <t>Während des Betriebes ist vom Kunde darauf zu achten, dass die Umgebungstemperaturen die angegebenen Extremwerte von -10°C bis +40°C nicht über- bzw unterschreiten. Außerdem sollte der Bandförderer nur von befugtem Personal betrieben werden.</t>
-  </si>
-  <si>
-    <t>Sollte das Förderband durch den Betrieb verschmutzt worden sein, sollten keine chemikalischen Reinigungsmittel verwendet werden, da das Material des Förderbandes, der Elekromotor oder andere Teile des Bandförderers dadurch beschädigt werden könnten. Sollte bei der Reinigung der Anlage eine Demontage einzelner Bestandteile notwendig sein ist die Demontage- und anschließend die Montageanleitung zu beachten. Bei Nichtbeachten kann die Funktion der Maschine nicht mehr gewährleistet werden.</t>
-  </si>
-  <si>
-    <t>Bei der Instanthaltung und Wartung ist darauf zu achten, dass dies durch qualifiziertes Personal erfolgt.</t>
-  </si>
-  <si>
     <t>Wird das Produkt außer Betrieb genommen oder demontiert, muss die Demontageanleitung beachtet werden.</t>
+  </si>
+  <si>
+    <t>Bei der Instandhaltung und Wartung ist darauf zu achten, dass dies durch qualifiziertes Personal erfolgt.</t>
+  </si>
+  <si>
+    <t>Während der ersten Lebensphase, der Produktion / Montage des Bandförderers, sind Mitarbeiter der Fertigung und Montage in direktem Kontakt mit dem Produkt. Eigenangefertige Teile können fehlerhaft produziert werden. Zukaufteile können ebenso fehlerhaft produziert, bestellt oder beim Transport beschädigt worden sein. Die Richtigkeit der Teile ist deshalb zu überprüfen.</t>
+  </si>
+  <si>
+    <t>Ebenso der Transport zum Kunden stellt ein hohes Risiko für Transportschäden dar. Das Produkt kann unter Umständen nicht fristgerecht geliefert werden oder Bestandteile davon könnten fehlen.</t>
+  </si>
+  <si>
+    <t>Während des Betriebes ist vom Kunden darauf zu achten, dass die Umgebungstemperaturen die angegebenen Extremwerte von -10°C bis +40°C nicht über- bzw. unterschreiten. Außerdem sollte der Bandförderer nur von befugtem Personal betrieben werden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das Personal sollte neben den grundsätzlichen Verhaltensweisen an Förderanlagen vor allem mit folgenden Hinweisen vertraut gemacht werden: Weite Kleidung oder offene Hare dürfen sich nicht im Einzugbereich der Trommel, der Welle oder des Bandes befinden. Das Band ist nicht als Personentransport oder zum Transport anderer Teile als denen des Stückgutes vorgesehen. Das Band sollte im laufenden Betrieb nicht mit der bloßen Hand berührt werden. </t>
+  </si>
+  <si>
+    <t>Sollte das Förderband durch den Betrieb verschmutzt worden sein, sollten keine chemikalischen Reinigungsmittel verwendet werden, da das Material des Förderbandes, der Elekromotor oder andere Teile des Bandförderers dadurch beschädigt werden könnten. Bei der Reinigung mit Wasser ist zu beachten, dass keine Wasserrücktände in den Ritzen verbleiben sollten. Sollte bei der Reinigung der Anlage eine Demontage einzelner Bestandteile notwendig sein, ist die Demontage- und anschließend die Montageanleitung zu beachten. Bei Nichtbeachten kann die Funktion der Maschine nicht mehr gewährleistet werden.</t>
+  </si>
+  <si>
+    <t>Der Bandförderer kann sowohl in einer Halle als auch draußen genutzt werden. Der Elektromotor darf allerdings nicht dauerhaft der Witterung ausgesetzt sein, sondern benötigt dann eine Abschirmung.</t>
+  </si>
+  <si>
+    <t>Die Lebensdauer beträgt 30000h, bedingt vor allem durch die Kugellager.</t>
+  </si>
+  <si>
+    <t>Steigung bis zu 3%</t>
+  </si>
+  <si>
+    <t>Bandbreite 240mm</t>
+  </si>
+  <si>
+    <t>Zur Einrichtung und zum Aufziehen des Bandes kann ein langsamer Betriebsmodus ausgewählt werden.</t>
+  </si>
+  <si>
+    <t>Im Standardbetrieb läuft das Band kontinuierlich mit einer Geschwindigkeit von ca. 2 m/s um.</t>
+  </si>
+  <si>
+    <t>Im Falle einer Störung kann das Band in langsamer Geschwindigkeit invertiert betrieben werden. Diese Betriebsstufe darf nur kurzfristig gewählt werden.</t>
+  </si>
+  <si>
+    <t>Durch die stufenlose Regelung der Geschwindigkeit und den damit verbundenen leistungsstarken Elektromotor kann das Förderband auch individuell an den Betrieb angepasst werden.</t>
+  </si>
+  <si>
+    <t>Der Bandförderer dient dem Transport von leichten bis mittelschweren Stückgütern auf waagerechtem oder leicht steigendem Untergrund. Die Güter werden auf das sich bewegende Band gelegt und vom Bandanfang bis Bandende transportiert. Das Band wird von einer Antriebsrolle angetrieben und von einer Gegenrolle umgelenkt. Die Bandrolle wird von einem Elektromotor angetrieben.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
     <numFmt numFmtId="165" formatCode="mmm\-yy"/>
@@ -2809,7 +2825,7 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="351">
+  <cellXfs count="354">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3435,6 +3451,93 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
@@ -3447,86 +3550,6 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3560,11 +3583,92 @@
     <xf numFmtId="49" fontId="22" fillId="3" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3593,93 +3697,12 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3695,6 +3718,15 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3731,24 +3763,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3770,58 +3829,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
-    <cellStyle name="Standard 3" xfId="2"/>
-    <cellStyle name="Standard 4" xfId="3"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standard 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -3950,7 +3978,7 @@
         <xdr:cNvPr id="2049" name="Text Box 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3972,14 +4000,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4049,7 +4077,7 @@
         <xdr:cNvPr id="2052" name="Text Box 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4071,14 +4099,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4453,11 +4481,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:L72"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4472,403 +4500,415 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25">
-      <c r="A1" s="238" t="s">
-        <v>433</v>
-      </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="239"/>
-      <c r="I1" s="239"/>
-      <c r="J1" s="239"/>
-      <c r="K1" s="239"/>
-      <c r="L1" s="240"/>
+      <c r="A1" s="260" t="s">
+        <v>432</v>
+      </c>
+      <c r="B1" s="261"/>
+      <c r="C1" s="261"/>
+      <c r="D1" s="261"/>
+      <c r="E1" s="261"/>
+      <c r="F1" s="261"/>
+      <c r="G1" s="261"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="261"/>
+      <c r="J1" s="261"/>
+      <c r="K1" s="261"/>
+      <c r="L1" s="262"/>
     </row>
     <row r="2" spans="1:12" ht="7.5" customHeight="1">
-      <c r="A2" s="245"/>
-      <c r="B2" s="246"/>
-      <c r="C2" s="246"/>
-      <c r="D2" s="246"/>
-      <c r="E2" s="246"/>
-      <c r="F2" s="246"/>
-      <c r="G2" s="246"/>
-      <c r="H2" s="246"/>
-      <c r="I2" s="246"/>
-      <c r="J2" s="246"/>
-      <c r="K2" s="246"/>
-      <c r="L2" s="247"/>
+      <c r="A2" s="247"/>
+      <c r="B2" s="248"/>
+      <c r="C2" s="248"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="248"/>
+      <c r="F2" s="248"/>
+      <c r="G2" s="248"/>
+      <c r="H2" s="248"/>
+      <c r="I2" s="248"/>
+      <c r="J2" s="248"/>
+      <c r="K2" s="248"/>
+      <c r="L2" s="249"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="248" t="s">
+      <c r="A3" s="243" t="s">
         <v>419</v>
       </c>
-      <c r="B3" s="249"/>
-      <c r="C3" s="249"/>
-      <c r="D3" s="249"/>
-      <c r="E3" s="249"/>
-      <c r="F3" s="249"/>
-      <c r="G3" s="249"/>
-      <c r="H3" s="249"/>
-      <c r="I3" s="249"/>
-      <c r="J3" s="249"/>
-      <c r="K3" s="249"/>
-      <c r="L3" s="250"/>
+      <c r="B3" s="244"/>
+      <c r="C3" s="244"/>
+      <c r="D3" s="244"/>
+      <c r="E3" s="244"/>
+      <c r="F3" s="244"/>
+      <c r="G3" s="244"/>
+      <c r="H3" s="244"/>
+      <c r="I3" s="244"/>
+      <c r="J3" s="244"/>
+      <c r="K3" s="244"/>
+      <c r="L3" s="245"/>
     </row>
     <row r="4" spans="1:12" ht="29.25" customHeight="1">
-      <c r="A4" s="244" t="s">
-        <v>443</v>
-      </c>
-      <c r="B4" s="242"/>
-      <c r="C4" s="242"/>
-      <c r="D4" s="242"/>
-      <c r="E4" s="242"/>
-      <c r="F4" s="242"/>
-      <c r="G4" s="242"/>
-      <c r="H4" s="242"/>
-      <c r="I4" s="242"/>
-      <c r="J4" s="242"/>
-      <c r="K4" s="242"/>
-      <c r="L4" s="243"/>
+      <c r="A4" s="246" t="s">
+        <v>454</v>
+      </c>
+      <c r="B4" s="241"/>
+      <c r="C4" s="241"/>
+      <c r="D4" s="241"/>
+      <c r="E4" s="241"/>
+      <c r="F4" s="241"/>
+      <c r="G4" s="241"/>
+      <c r="H4" s="241"/>
+      <c r="I4" s="241"/>
+      <c r="J4" s="241"/>
+      <c r="K4" s="241"/>
+      <c r="L4" s="242"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="241"/>
-      <c r="B5" s="242"/>
-      <c r="C5" s="242"/>
-      <c r="D5" s="242"/>
-      <c r="E5" s="242"/>
-      <c r="F5" s="242"/>
-      <c r="G5" s="242"/>
-      <c r="H5" s="242"/>
-      <c r="I5" s="242"/>
-      <c r="J5" s="242"/>
-      <c r="K5" s="242"/>
-      <c r="L5" s="243"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="244"/>
-      <c r="B6" s="242"/>
-      <c r="C6" s="242"/>
-      <c r="D6" s="242"/>
-      <c r="E6" s="242"/>
-      <c r="F6" s="242"/>
-      <c r="G6" s="242"/>
-      <c r="H6" s="242"/>
-      <c r="I6" s="242"/>
-      <c r="J6" s="242"/>
-      <c r="K6" s="242"/>
-      <c r="L6" s="243"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="241"/>
-      <c r="B7" s="242"/>
-      <c r="C7" s="242"/>
-      <c r="D7" s="242"/>
-      <c r="E7" s="242"/>
-      <c r="F7" s="242"/>
-      <c r="G7" s="242"/>
-      <c r="H7" s="242"/>
-      <c r="I7" s="242"/>
-      <c r="J7" s="242"/>
-      <c r="K7" s="242"/>
-      <c r="L7" s="243"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75">
-      <c r="A8" s="255" t="s">
+      <c r="A5" s="240"/>
+      <c r="B5" s="241"/>
+      <c r="C5" s="241"/>
+      <c r="D5" s="241"/>
+      <c r="E5" s="241"/>
+      <c r="F5" s="241"/>
+      <c r="G5" s="241"/>
+      <c r="H5" s="241"/>
+      <c r="I5" s="241"/>
+      <c r="J5" s="241"/>
+      <c r="K5" s="241"/>
+      <c r="L5" s="242"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75">
+      <c r="A6" s="253" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="249"/>
-      <c r="C8" s="249"/>
-      <c r="D8" s="249"/>
-      <c r="E8" s="249"/>
-      <c r="F8" s="249"/>
-      <c r="G8" s="249"/>
-      <c r="H8" s="249"/>
-      <c r="I8" s="249"/>
-      <c r="J8" s="249"/>
-      <c r="K8" s="249"/>
-      <c r="L8" s="250"/>
-    </row>
-    <row r="9" spans="1:12" ht="12.75" customHeight="1">
-      <c r="A9" s="244" t="s">
+      <c r="B6" s="244"/>
+      <c r="C6" s="244"/>
+      <c r="D6" s="244"/>
+      <c r="E6" s="244"/>
+      <c r="F6" s="244"/>
+      <c r="G6" s="244"/>
+      <c r="H6" s="244"/>
+      <c r="I6" s="244"/>
+      <c r="J6" s="244"/>
+      <c r="K6" s="244"/>
+      <c r="L6" s="245"/>
+    </row>
+    <row r="7" spans="1:12" ht="12.75" customHeight="1">
+      <c r="A7" s="353" t="s">
+        <v>450</v>
+      </c>
+      <c r="B7" s="353"/>
+      <c r="C7" s="353"/>
+      <c r="D7" s="353"/>
+      <c r="E7" s="353"/>
+      <c r="F7" s="353"/>
+      <c r="G7" s="353"/>
+      <c r="H7" s="353"/>
+      <c r="I7" s="353"/>
+      <c r="J7" s="353"/>
+      <c r="K7" s="353"/>
+      <c r="L7" s="353"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="246" t="s">
+        <v>451</v>
+      </c>
+      <c r="B8" s="241"/>
+      <c r="C8" s="241"/>
+      <c r="D8" s="241"/>
+      <c r="E8" s="241"/>
+      <c r="F8" s="241"/>
+      <c r="G8" s="241"/>
+      <c r="H8" s="241"/>
+      <c r="I8" s="241"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="241"/>
+      <c r="L8" s="242"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="246" t="s">
+        <v>452</v>
+      </c>
+      <c r="B9" s="351"/>
+      <c r="C9" s="351"/>
+      <c r="D9" s="351"/>
+      <c r="E9" s="351"/>
+      <c r="F9" s="351"/>
+      <c r="G9" s="351"/>
+      <c r="H9" s="351"/>
+      <c r="I9" s="351"/>
+      <c r="J9" s="351"/>
+      <c r="K9" s="351"/>
+      <c r="L9" s="352"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="246" t="s">
+        <v>453</v>
+      </c>
+      <c r="B10" s="241"/>
+      <c r="C10" s="241"/>
+      <c r="D10" s="241"/>
+      <c r="E10" s="241"/>
+      <c r="F10" s="241"/>
+      <c r="G10" s="241"/>
+      <c r="H10" s="241"/>
+      <c r="I10" s="241"/>
+      <c r="J10" s="241"/>
+      <c r="K10" s="241"/>
+      <c r="L10" s="242"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="240"/>
+      <c r="B11" s="241"/>
+      <c r="C11" s="241"/>
+      <c r="D11" s="241"/>
+      <c r="E11" s="241"/>
+      <c r="F11" s="241"/>
+      <c r="G11" s="241"/>
+      <c r="H11" s="241"/>
+      <c r="I11" s="241"/>
+      <c r="J11" s="241"/>
+      <c r="K11" s="241"/>
+      <c r="L11" s="242"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75">
+      <c r="A12" s="253" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="244"/>
+      <c r="C12" s="244"/>
+      <c r="D12" s="244"/>
+      <c r="E12" s="244"/>
+      <c r="F12" s="244"/>
+      <c r="G12" s="244"/>
+      <c r="H12" s="244"/>
+      <c r="I12" s="244"/>
+      <c r="J12" s="244"/>
+      <c r="K12" s="244"/>
+      <c r="L12" s="245"/>
+    </row>
+    <row r="13" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A13" s="246" t="s">
+        <v>446</v>
+      </c>
+      <c r="B13" s="241"/>
+      <c r="C13" s="241"/>
+      <c r="D13" s="241"/>
+      <c r="E13" s="241"/>
+      <c r="F13" s="241"/>
+      <c r="G13" s="241"/>
+      <c r="H13" s="241"/>
+      <c r="I13" s="241"/>
+      <c r="J13" s="241"/>
+      <c r="K13" s="241"/>
+      <c r="L13" s="242"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="246" t="s">
         <v>431</v>
       </c>
-      <c r="B9" s="242"/>
-      <c r="C9" s="242"/>
-      <c r="D9" s="242"/>
-      <c r="E9" s="242"/>
-      <c r="F9" s="242"/>
-      <c r="G9" s="242"/>
-      <c r="H9" s="242"/>
-      <c r="I9" s="242"/>
-      <c r="J9" s="242"/>
-      <c r="K9" s="242"/>
-      <c r="L9" s="243"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="241"/>
-      <c r="B10" s="242"/>
-      <c r="C10" s="242"/>
-      <c r="D10" s="242"/>
-      <c r="E10" s="242"/>
-      <c r="F10" s="242"/>
-      <c r="G10" s="242"/>
-      <c r="H10" s="242"/>
-      <c r="I10" s="242"/>
-      <c r="J10" s="242"/>
-      <c r="K10" s="242"/>
-      <c r="L10" s="243"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="241"/>
-      <c r="B11" s="242"/>
-      <c r="C11" s="242"/>
-      <c r="D11" s="242"/>
-      <c r="E11" s="242"/>
-      <c r="F11" s="242"/>
-      <c r="G11" s="242"/>
-      <c r="H11" s="242"/>
-      <c r="I11" s="242"/>
-      <c r="J11" s="242"/>
-      <c r="K11" s="242"/>
-      <c r="L11" s="243"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="241"/>
-      <c r="B12" s="242"/>
-      <c r="C12" s="242"/>
-      <c r="D12" s="242"/>
-      <c r="E12" s="242"/>
-      <c r="F12" s="242"/>
-      <c r="G12" s="242"/>
-      <c r="H12" s="242"/>
-      <c r="I12" s="242"/>
-      <c r="J12" s="242"/>
-      <c r="K12" s="242"/>
-      <c r="L12" s="243"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75">
-      <c r="A13" s="255" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="249"/>
-      <c r="C13" s="249"/>
-      <c r="D13" s="249"/>
-      <c r="E13" s="249"/>
-      <c r="F13" s="249"/>
-      <c r="G13" s="249"/>
-      <c r="H13" s="249"/>
-      <c r="I13" s="249"/>
-      <c r="J13" s="249"/>
-      <c r="K13" s="249"/>
-      <c r="L13" s="250"/>
-    </row>
-    <row r="14" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A14" s="244" t="s">
-        <v>437</v>
-      </c>
-      <c r="B14" s="242"/>
-      <c r="C14" s="242"/>
-      <c r="D14" s="242"/>
-      <c r="E14" s="242"/>
-      <c r="F14" s="242"/>
-      <c r="G14" s="242"/>
-      <c r="H14" s="242"/>
-      <c r="I14" s="242"/>
-      <c r="J14" s="242"/>
-      <c r="K14" s="242"/>
-      <c r="L14" s="243"/>
+      <c r="B14" s="241"/>
+      <c r="C14" s="241"/>
+      <c r="D14" s="241"/>
+      <c r="E14" s="241"/>
+      <c r="F14" s="241"/>
+      <c r="G14" s="241"/>
+      <c r="H14" s="241"/>
+      <c r="I14" s="241"/>
+      <c r="J14" s="241"/>
+      <c r="K14" s="241"/>
+      <c r="L14" s="242"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="244" t="s">
-        <v>432</v>
-      </c>
-      <c r="B15" s="242"/>
-      <c r="C15" s="242"/>
-      <c r="D15" s="242"/>
-      <c r="E15" s="242"/>
-      <c r="F15" s="242"/>
-      <c r="G15" s="242"/>
-      <c r="H15" s="242"/>
-      <c r="I15" s="242"/>
-      <c r="J15" s="242"/>
-      <c r="K15" s="242"/>
-      <c r="L15" s="243"/>
+      <c r="A15" s="246"/>
+      <c r="B15" s="241"/>
+      <c r="C15" s="241"/>
+      <c r="D15" s="241"/>
+      <c r="E15" s="241"/>
+      <c r="F15" s="241"/>
+      <c r="G15" s="241"/>
+      <c r="H15" s="241"/>
+      <c r="I15" s="241"/>
+      <c r="J15" s="241"/>
+      <c r="K15" s="241"/>
+      <c r="L15" s="242"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="244"/>
-      <c r="B16" s="242"/>
-      <c r="C16" s="242"/>
-      <c r="D16" s="242"/>
-      <c r="E16" s="242"/>
-      <c r="F16" s="242"/>
-      <c r="G16" s="242"/>
-      <c r="H16" s="242"/>
-      <c r="I16" s="242"/>
-      <c r="J16" s="242"/>
-      <c r="K16" s="242"/>
-      <c r="L16" s="243"/>
+      <c r="A16" s="240"/>
+      <c r="B16" s="241"/>
+      <c r="C16" s="241"/>
+      <c r="D16" s="241"/>
+      <c r="E16" s="241"/>
+      <c r="F16" s="241"/>
+      <c r="G16" s="241"/>
+      <c r="H16" s="241"/>
+      <c r="I16" s="241"/>
+      <c r="J16" s="241"/>
+      <c r="K16" s="241"/>
+      <c r="L16" s="242"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="241"/>
-      <c r="B17" s="242"/>
-      <c r="C17" s="242"/>
-      <c r="D17" s="242"/>
-      <c r="E17" s="242"/>
-      <c r="F17" s="242"/>
-      <c r="G17" s="242"/>
-      <c r="H17" s="242"/>
-      <c r="I17" s="242"/>
-      <c r="J17" s="242"/>
-      <c r="K17" s="242"/>
-      <c r="L17" s="243"/>
+      <c r="A17" s="240"/>
+      <c r="B17" s="241"/>
+      <c r="C17" s="241"/>
+      <c r="D17" s="241"/>
+      <c r="E17" s="241"/>
+      <c r="F17" s="241"/>
+      <c r="G17" s="241"/>
+      <c r="H17" s="241"/>
+      <c r="I17" s="241"/>
+      <c r="J17" s="241"/>
+      <c r="K17" s="241"/>
+      <c r="L17" s="242"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="241"/>
-      <c r="B18" s="242"/>
-      <c r="C18" s="242"/>
-      <c r="D18" s="242"/>
-      <c r="E18" s="242"/>
-      <c r="F18" s="242"/>
-      <c r="G18" s="242"/>
-      <c r="H18" s="242"/>
-      <c r="I18" s="242"/>
-      <c r="J18" s="242"/>
-      <c r="K18" s="242"/>
-      <c r="L18" s="243"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="241"/>
-      <c r="B19" s="242"/>
-      <c r="C19" s="242"/>
-      <c r="D19" s="242"/>
-      <c r="E19" s="242"/>
-      <c r="F19" s="242"/>
-      <c r="G19" s="242"/>
-      <c r="H19" s="242"/>
-      <c r="I19" s="242"/>
-      <c r="J19" s="242"/>
-      <c r="K19" s="242"/>
-      <c r="L19" s="243"/>
-    </row>
-    <row r="20" spans="1:13" ht="6" customHeight="1">
-      <c r="A20" s="245"/>
-      <c r="B20" s="246"/>
-      <c r="C20" s="246"/>
-      <c r="D20" s="246"/>
-      <c r="E20" s="246"/>
-      <c r="F20" s="246"/>
-      <c r="G20" s="246"/>
-      <c r="H20" s="246"/>
-      <c r="I20" s="246"/>
-      <c r="J20" s="246"/>
-      <c r="K20" s="246"/>
-      <c r="L20" s="247"/>
-    </row>
-    <row r="21" spans="1:13" ht="15.75">
-      <c r="A21" s="248" t="s">
+      <c r="A18" s="240"/>
+      <c r="B18" s="241"/>
+      <c r="C18" s="241"/>
+      <c r="D18" s="241"/>
+      <c r="E18" s="241"/>
+      <c r="F18" s="241"/>
+      <c r="G18" s="241"/>
+      <c r="H18" s="241"/>
+      <c r="I18" s="241"/>
+      <c r="J18" s="241"/>
+      <c r="K18" s="241"/>
+      <c r="L18" s="242"/>
+    </row>
+    <row r="19" spans="1:13" ht="6" customHeight="1">
+      <c r="A19" s="247"/>
+      <c r="B19" s="248"/>
+      <c r="C19" s="248"/>
+      <c r="D19" s="248"/>
+      <c r="E19" s="248"/>
+      <c r="F19" s="248"/>
+      <c r="G19" s="248"/>
+      <c r="H19" s="248"/>
+      <c r="I19" s="248"/>
+      <c r="J19" s="248"/>
+      <c r="K19" s="248"/>
+      <c r="L19" s="249"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75">
+      <c r="A20" s="243" t="s">
         <v>393</v>
       </c>
-      <c r="B21" s="249"/>
-      <c r="C21" s="249"/>
-      <c r="D21" s="249"/>
-      <c r="E21" s="249"/>
-      <c r="F21" s="249"/>
-      <c r="G21" s="249"/>
-      <c r="H21" s="249"/>
-      <c r="I21" s="249"/>
-      <c r="J21" s="249"/>
-      <c r="K21" s="249"/>
-      <c r="L21" s="250"/>
+      <c r="B20" s="244"/>
+      <c r="C20" s="244"/>
+      <c r="D20" s="244"/>
+      <c r="E20" s="244"/>
+      <c r="F20" s="244"/>
+      <c r="G20" s="244"/>
+      <c r="H20" s="244"/>
+      <c r="I20" s="244"/>
+      <c r="J20" s="244"/>
+      <c r="K20" s="244"/>
+      <c r="L20" s="245"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="246"/>
+      <c r="B21" s="257"/>
+      <c r="C21" s="257"/>
+      <c r="D21" s="257"/>
+      <c r="E21" s="257"/>
+      <c r="F21" s="257"/>
+      <c r="G21" s="257"/>
+      <c r="H21" s="257"/>
+      <c r="I21" s="257"/>
+      <c r="J21" s="257"/>
+      <c r="K21" s="257"/>
+      <c r="L21" s="242"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="244"/>
-      <c r="B22" s="257"/>
-      <c r="C22" s="257"/>
-      <c r="D22" s="257"/>
-      <c r="E22" s="257"/>
-      <c r="F22" s="257"/>
-      <c r="G22" s="257"/>
-      <c r="H22" s="257"/>
-      <c r="I22" s="257"/>
-      <c r="J22" s="257"/>
-      <c r="K22" s="257"/>
-      <c r="L22" s="243"/>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="253"/>
-      <c r="B23" s="256" t="s">
+      <c r="A22" s="258"/>
+      <c r="B22" s="254" t="s">
         <v>370</v>
       </c>
-      <c r="C23" s="256"/>
-      <c r="D23" s="256"/>
-      <c r="E23" s="256"/>
-      <c r="F23" s="256"/>
-      <c r="G23" s="256"/>
-      <c r="H23" s="256"/>
-      <c r="I23" s="256"/>
-      <c r="J23" s="256"/>
-      <c r="K23" s="256"/>
-      <c r="L23" s="135"/>
-      <c r="M23" s="137"/>
-    </row>
-    <row r="24" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A24" s="254"/>
-      <c r="B24" s="251" t="s">
+      <c r="C22" s="254"/>
+      <c r="D22" s="254"/>
+      <c r="E22" s="254"/>
+      <c r="F22" s="254"/>
+      <c r="G22" s="254"/>
+      <c r="H22" s="254"/>
+      <c r="I22" s="254"/>
+      <c r="J22" s="254"/>
+      <c r="K22" s="254"/>
+      <c r="L22" s="135"/>
+      <c r="M22" s="137"/>
+    </row>
+    <row r="23" spans="1:13" ht="12.75" customHeight="1">
+      <c r="A23" s="259"/>
+      <c r="B23" s="255" t="s">
         <v>376</v>
       </c>
-      <c r="C24" s="251" t="s">
+      <c r="C23" s="255" t="s">
         <v>378</v>
       </c>
-      <c r="D24" s="251" t="s">
+      <c r="D23" s="255" t="s">
         <v>373</v>
       </c>
-      <c r="E24" s="251" t="s">
+      <c r="E23" s="255" t="s">
         <v>375</v>
       </c>
-      <c r="F24" s="251" t="s">
+      <c r="F23" s="255" t="s">
         <v>371</v>
       </c>
-      <c r="G24" s="251" t="s">
+      <c r="G23" s="255" t="s">
         <v>377</v>
       </c>
-      <c r="H24" s="251" t="s">
+      <c r="H23" s="255" t="s">
         <v>374</v>
       </c>
-      <c r="I24" s="251" t="s">
+      <c r="I23" s="255" t="s">
         <v>379</v>
       </c>
-      <c r="J24" s="251"/>
-      <c r="K24" s="251"/>
+      <c r="J23" s="255"/>
+      <c r="K23" s="255"/>
+      <c r="L23" s="136"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="133" t="s">
+        <v>391</v>
+      </c>
+      <c r="B24" s="256"/>
+      <c r="C24" s="256"/>
+      <c r="D24" s="256"/>
+      <c r="E24" s="256"/>
+      <c r="F24" s="256"/>
+      <c r="G24" s="256"/>
+      <c r="H24" s="256"/>
+      <c r="I24" s="256"/>
+      <c r="J24" s="256"/>
+      <c r="K24" s="256"/>
       <c r="L24" s="136"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="133" t="s">
-        <v>391</v>
-      </c>
-      <c r="B25" s="252"/>
-      <c r="C25" s="252"/>
-      <c r="D25" s="252"/>
-      <c r="E25" s="252"/>
-      <c r="F25" s="252"/>
-      <c r="G25" s="252"/>
-      <c r="H25" s="252"/>
-      <c r="I25" s="252"/>
-      <c r="J25" s="252"/>
-      <c r="K25" s="252"/>
+      <c r="A25" s="238" t="s">
+        <v>410</v>
+      </c>
+      <c r="B25" s="239" t="s">
+        <v>366</v>
+      </c>
+      <c r="C25" s="239"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="134"/>
+      <c r="H25" s="134"/>
+      <c r="I25" s="134"/>
+      <c r="J25" s="134"/>
+      <c r="K25" s="134"/>
       <c r="L25" s="136"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="349" t="s">
-        <v>410</v>
-      </c>
-      <c r="B26" s="350" t="s">
+      <c r="A26" t="s">
+        <v>407</v>
+      </c>
+      <c r="B26" s="134"/>
+      <c r="C26" s="239" t="s">
         <v>366</v>
       </c>
-      <c r="C26" s="350"/>
-      <c r="D26" s="134"/>
+      <c r="D26" s="239" t="s">
+        <v>366</v>
+      </c>
       <c r="E26" s="134"/>
       <c r="F26" s="134"/>
       <c r="G26" s="134"/>
@@ -4880,17 +4920,15 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B27" s="134"/>
-      <c r="C27" s="350" t="s">
+      <c r="C27" s="134"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="239" t="s">
         <v>366</v>
       </c>
-      <c r="D27" s="350" t="s">
-        <v>366</v>
-      </c>
-      <c r="E27" s="134"/>
-      <c r="F27" s="134"/>
+      <c r="F27" s="239"/>
       <c r="G27" s="134"/>
       <c r="H27" s="134"/>
       <c r="I27" s="134"/>
@@ -4900,15 +4938,15 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B28" s="134"/>
       <c r="C28" s="134"/>
       <c r="D28" s="134"/>
-      <c r="E28" s="350" t="s">
+      <c r="E28" s="134"/>
+      <c r="F28" s="239" t="s">
         <v>366</v>
       </c>
-      <c r="F28" s="350"/>
       <c r="G28" s="134"/>
       <c r="H28" s="134"/>
       <c r="I28" s="134"/>
@@ -4918,13 +4956,13 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B29" s="134"/>
       <c r="C29" s="134"/>
       <c r="D29" s="134"/>
       <c r="E29" s="134"/>
-      <c r="F29" s="350" t="s">
+      <c r="F29" s="239" t="s">
         <v>366</v>
       </c>
       <c r="G29" s="134"/>
@@ -4936,13 +4974,13 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B30" s="134"/>
       <c r="C30" s="134"/>
       <c r="D30" s="134"/>
       <c r="E30" s="134"/>
-      <c r="F30" s="350" t="s">
+      <c r="F30" s="239" t="s">
         <v>366</v>
       </c>
       <c r="G30" s="134"/>
@@ -4954,13 +4992,13 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B31" s="134"/>
       <c r="C31" s="134"/>
       <c r="D31" s="134"/>
       <c r="E31" s="134"/>
-      <c r="F31" s="350" t="s">
+      <c r="F31" s="239" t="s">
         <v>366</v>
       </c>
       <c r="G31" s="134"/>
@@ -4972,13 +5010,13 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B32" s="134"/>
       <c r="C32" s="134"/>
       <c r="D32" s="134"/>
       <c r="E32" s="134"/>
-      <c r="F32" s="350" t="s">
+      <c r="F32" s="239" t="s">
         <v>366</v>
       </c>
       <c r="G32" s="134"/>
@@ -4990,17 +5028,19 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B33" s="134"/>
       <c r="C33" s="134"/>
       <c r="D33" s="134"/>
       <c r="E33" s="134"/>
-      <c r="F33" s="350" t="s">
+      <c r="F33" s="239" t="s">
         <v>366</v>
       </c>
-      <c r="G33" s="134"/>
-      <c r="H33" s="134"/>
+      <c r="G33" s="239" t="s">
+        <v>366</v>
+      </c>
+      <c r="H33" s="239"/>
       <c r="I33" s="134"/>
       <c r="J33" s="134"/>
       <c r="K33" s="134"/>
@@ -5008,19 +5048,21 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B34" s="134"/>
       <c r="C34" s="134"/>
       <c r="D34" s="134"/>
-      <c r="E34" s="134"/>
-      <c r="F34" s="350" t="s">
+      <c r="E34" s="239" t="s">
         <v>366</v>
       </c>
-      <c r="G34" s="350" t="s">
+      <c r="F34" s="134"/>
+      <c r="G34" s="239" t="s">
         <v>366</v>
       </c>
-      <c r="H34" s="350"/>
+      <c r="H34" s="239" t="s">
+        <v>366</v>
+      </c>
       <c r="I34" s="134"/>
       <c r="J34" s="134"/>
       <c r="K34" s="134"/>
@@ -5028,667 +5070,663 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B35" s="134"/>
       <c r="C35" s="134"/>
       <c r="D35" s="134"/>
-      <c r="E35" s="350" t="s">
+      <c r="E35" s="134"/>
+      <c r="F35" s="239" t="s">
         <v>366</v>
       </c>
-      <c r="F35" s="134"/>
-      <c r="G35" s="350" t="s">
+      <c r="G35" s="134"/>
+      <c r="H35" s="134"/>
+      <c r="I35" s="239" t="s">
         <v>366</v>
       </c>
-      <c r="H35" s="350" t="s">
-        <v>366</v>
-      </c>
-      <c r="I35" s="134"/>
       <c r="J35" s="134"/>
       <c r="K35" s="134"/>
       <c r="L35" s="136"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" t="s">
-        <v>417</v>
-      </c>
-      <c r="B36" s="134"/>
-      <c r="C36" s="134"/>
-      <c r="D36" s="134"/>
-      <c r="E36" s="134"/>
-      <c r="F36" s="350" t="s">
-        <v>366</v>
-      </c>
-      <c r="G36" s="134"/>
-      <c r="H36" s="134"/>
-      <c r="I36" s="350" t="s">
-        <v>366</v>
-      </c>
-      <c r="J36" s="134"/>
-      <c r="K36" s="134"/>
-      <c r="L36" s="136"/>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="241"/>
-      <c r="B37" s="242"/>
-      <c r="C37" s="242"/>
-      <c r="D37" s="242"/>
-      <c r="E37" s="242"/>
-      <c r="F37" s="242"/>
-      <c r="G37" s="242"/>
-      <c r="H37" s="242"/>
-      <c r="I37" s="242"/>
-      <c r="J37" s="242"/>
-      <c r="K37" s="242"/>
-      <c r="L37" s="243"/>
-    </row>
-    <row r="38" spans="1:12" ht="12.75" customHeight="1">
-      <c r="A38" s="241" t="s">
+      <c r="A36" s="240"/>
+      <c r="B36" s="241"/>
+      <c r="C36" s="241"/>
+      <c r="D36" s="241"/>
+      <c r="E36" s="241"/>
+      <c r="F36" s="241"/>
+      <c r="G36" s="241"/>
+      <c r="H36" s="241"/>
+      <c r="I36" s="241"/>
+      <c r="J36" s="241"/>
+      <c r="K36" s="241"/>
+      <c r="L36" s="242"/>
+    </row>
+    <row r="37" spans="1:12" ht="12.75" customHeight="1">
+      <c r="A37" s="240" t="s">
         <v>372</v>
       </c>
-      <c r="B38" s="242"/>
-      <c r="C38" s="242"/>
-      <c r="D38" s="242"/>
-      <c r="E38" s="242"/>
-      <c r="F38" s="242"/>
-      <c r="G38" s="242"/>
-      <c r="H38" s="242"/>
-      <c r="I38" s="242"/>
-      <c r="J38" s="242"/>
-      <c r="K38" s="242"/>
-      <c r="L38" s="243"/>
+      <c r="B37" s="241"/>
+      <c r="C37" s="241"/>
+      <c r="D37" s="241"/>
+      <c r="E37" s="241"/>
+      <c r="F37" s="241"/>
+      <c r="G37" s="241"/>
+      <c r="H37" s="241"/>
+      <c r="I37" s="241"/>
+      <c r="J37" s="241"/>
+      <c r="K37" s="241"/>
+      <c r="L37" s="242"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="246" t="s">
+        <v>420</v>
+      </c>
+      <c r="B38" s="241"/>
+      <c r="C38" s="241"/>
+      <c r="D38" s="241"/>
+      <c r="E38" s="241"/>
+      <c r="F38" s="241"/>
+      <c r="G38" s="241"/>
+      <c r="H38" s="241"/>
+      <c r="I38" s="241"/>
+      <c r="J38" s="241"/>
+      <c r="K38" s="241"/>
+      <c r="L38" s="242"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="244" t="s">
-        <v>420</v>
-      </c>
-      <c r="B39" s="242"/>
-      <c r="C39" s="242"/>
-      <c r="D39" s="242"/>
-      <c r="E39" s="242"/>
-      <c r="F39" s="242"/>
-      <c r="G39" s="242"/>
-      <c r="H39" s="242"/>
-      <c r="I39" s="242"/>
-      <c r="J39" s="242"/>
-      <c r="K39" s="242"/>
-      <c r="L39" s="243"/>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="241"/>
-      <c r="B40" s="242"/>
-      <c r="C40" s="242"/>
-      <c r="D40" s="242"/>
-      <c r="E40" s="242"/>
-      <c r="F40" s="242"/>
-      <c r="G40" s="242"/>
-      <c r="H40" s="242"/>
-      <c r="I40" s="242"/>
-      <c r="J40" s="242"/>
-      <c r="K40" s="242"/>
-      <c r="L40" s="243"/>
-    </row>
-    <row r="41" spans="1:12" ht="6" customHeight="1">
-      <c r="A41" s="245"/>
-      <c r="B41" s="246"/>
-      <c r="C41" s="246"/>
-      <c r="D41" s="246"/>
-      <c r="E41" s="246"/>
-      <c r="F41" s="246"/>
-      <c r="G41" s="246"/>
-      <c r="H41" s="246"/>
-      <c r="I41" s="246"/>
-      <c r="J41" s="246"/>
-      <c r="K41" s="246"/>
-      <c r="L41" s="247"/>
-    </row>
-    <row r="42" spans="1:12" ht="15.75">
-      <c r="A42" s="248" t="s">
+      <c r="A39" s="240"/>
+      <c r="B39" s="241"/>
+      <c r="C39" s="241"/>
+      <c r="D39" s="241"/>
+      <c r="E39" s="241"/>
+      <c r="F39" s="241"/>
+      <c r="G39" s="241"/>
+      <c r="H39" s="241"/>
+      <c r="I39" s="241"/>
+      <c r="J39" s="241"/>
+      <c r="K39" s="241"/>
+      <c r="L39" s="242"/>
+    </row>
+    <row r="40" spans="1:12" ht="6" customHeight="1">
+      <c r="A40" s="247"/>
+      <c r="B40" s="248"/>
+      <c r="C40" s="248"/>
+      <c r="D40" s="248"/>
+      <c r="E40" s="248"/>
+      <c r="F40" s="248"/>
+      <c r="G40" s="248"/>
+      <c r="H40" s="248"/>
+      <c r="I40" s="248"/>
+      <c r="J40" s="248"/>
+      <c r="K40" s="248"/>
+      <c r="L40" s="249"/>
+    </row>
+    <row r="41" spans="1:12" ht="15.75">
+      <c r="A41" s="243" t="s">
         <v>421</v>
       </c>
-      <c r="B42" s="249"/>
-      <c r="C42" s="249"/>
-      <c r="D42" s="249"/>
-      <c r="E42" s="249"/>
-      <c r="F42" s="249"/>
-      <c r="G42" s="249"/>
-      <c r="H42" s="249"/>
-      <c r="I42" s="249"/>
-      <c r="J42" s="249"/>
-      <c r="K42" s="249"/>
-      <c r="L42" s="250"/>
+      <c r="B41" s="244"/>
+      <c r="C41" s="244"/>
+      <c r="D41" s="244"/>
+      <c r="E41" s="244"/>
+      <c r="F41" s="244"/>
+      <c r="G41" s="244"/>
+      <c r="H41" s="244"/>
+      <c r="I41" s="244"/>
+      <c r="J41" s="244"/>
+      <c r="K41" s="244"/>
+      <c r="L41" s="245"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="246" t="s">
+        <v>433</v>
+      </c>
+      <c r="B42" s="241"/>
+      <c r="C42" s="241"/>
+      <c r="D42" s="241"/>
+      <c r="E42" s="241"/>
+      <c r="F42" s="241"/>
+      <c r="G42" s="241"/>
+      <c r="H42" s="241"/>
+      <c r="I42" s="241"/>
+      <c r="J42" s="241"/>
+      <c r="K42" s="241"/>
+      <c r="L42" s="242"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="244" t="s">
+      <c r="A43" s="246" t="s">
         <v>434</v>
       </c>
-      <c r="B43" s="242"/>
-      <c r="C43" s="242"/>
-      <c r="D43" s="242"/>
-      <c r="E43" s="242"/>
-      <c r="F43" s="242"/>
-      <c r="G43" s="242"/>
-      <c r="H43" s="242"/>
-      <c r="I43" s="242"/>
-      <c r="J43" s="242"/>
-      <c r="K43" s="242"/>
-      <c r="L43" s="243"/>
+      <c r="B43" s="241"/>
+      <c r="C43" s="241"/>
+      <c r="D43" s="241"/>
+      <c r="E43" s="241"/>
+      <c r="F43" s="241"/>
+      <c r="G43" s="241"/>
+      <c r="H43" s="241"/>
+      <c r="I43" s="241"/>
+      <c r="J43" s="241"/>
+      <c r="K43" s="241"/>
+      <c r="L43" s="242"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="244" t="s">
+      <c r="A44" s="240"/>
+      <c r="B44" s="241"/>
+      <c r="C44" s="241"/>
+      <c r="D44" s="241"/>
+      <c r="E44" s="241"/>
+      <c r="F44" s="241"/>
+      <c r="G44" s="241"/>
+      <c r="H44" s="241"/>
+      <c r="I44" s="241"/>
+      <c r="J44" s="241"/>
+      <c r="K44" s="241"/>
+      <c r="L44" s="242"/>
+    </row>
+    <row r="45" spans="1:12" ht="6" customHeight="1">
+      <c r="A45" s="247"/>
+      <c r="B45" s="248"/>
+      <c r="C45" s="248"/>
+      <c r="D45" s="248"/>
+      <c r="E45" s="248"/>
+      <c r="F45" s="248"/>
+      <c r="G45" s="248"/>
+      <c r="H45" s="248"/>
+      <c r="I45" s="248"/>
+      <c r="J45" s="248"/>
+      <c r="K45" s="248"/>
+      <c r="L45" s="249"/>
+    </row>
+    <row r="46" spans="1:12" ht="15.75">
+      <c r="A46" s="243" t="s">
+        <v>422</v>
+      </c>
+      <c r="B46" s="244"/>
+      <c r="C46" s="244"/>
+      <c r="D46" s="244"/>
+      <c r="E46" s="244"/>
+      <c r="F46" s="244"/>
+      <c r="G46" s="244"/>
+      <c r="H46" s="244"/>
+      <c r="I46" s="244"/>
+      <c r="J46" s="244"/>
+      <c r="K46" s="244"/>
+      <c r="L46" s="245"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="246" t="s">
+        <v>447</v>
+      </c>
+      <c r="B47" s="241"/>
+      <c r="C47" s="241"/>
+      <c r="D47" s="241"/>
+      <c r="E47" s="241"/>
+      <c r="F47" s="241"/>
+      <c r="G47" s="241"/>
+      <c r="H47" s="241"/>
+      <c r="I47" s="241"/>
+      <c r="J47" s="241"/>
+      <c r="K47" s="241"/>
+      <c r="L47" s="242"/>
+    </row>
+    <row r="48" spans="1:12" ht="6" customHeight="1">
+      <c r="A48" s="247"/>
+      <c r="B48" s="248"/>
+      <c r="C48" s="248"/>
+      <c r="D48" s="248"/>
+      <c r="E48" s="248"/>
+      <c r="F48" s="248"/>
+      <c r="G48" s="248"/>
+      <c r="H48" s="248"/>
+      <c r="I48" s="248"/>
+      <c r="J48" s="248"/>
+      <c r="K48" s="248"/>
+      <c r="L48" s="249"/>
+    </row>
+    <row r="49" spans="1:12" ht="15.75">
+      <c r="A49" s="243" t="s">
+        <v>423</v>
+      </c>
+      <c r="B49" s="244"/>
+      <c r="C49" s="244"/>
+      <c r="D49" s="244"/>
+      <c r="E49" s="244"/>
+      <c r="F49" s="244"/>
+      <c r="G49" s="244"/>
+      <c r="H49" s="244"/>
+      <c r="I49" s="244"/>
+      <c r="J49" s="244"/>
+      <c r="K49" s="244"/>
+      <c r="L49" s="245"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="246" t="s">
+        <v>430</v>
+      </c>
+      <c r="B50" s="241"/>
+      <c r="C50" s="241"/>
+      <c r="D50" s="241"/>
+      <c r="E50" s="241"/>
+      <c r="F50" s="241"/>
+      <c r="G50" s="241"/>
+      <c r="H50" s="241"/>
+      <c r="I50" s="241"/>
+      <c r="J50" s="241"/>
+      <c r="K50" s="241"/>
+      <c r="L50" s="242"/>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="246" t="s">
+        <v>448</v>
+      </c>
+      <c r="B51" s="241"/>
+      <c r="C51" s="241"/>
+      <c r="D51" s="241"/>
+      <c r="E51" s="241"/>
+      <c r="F51" s="241"/>
+      <c r="G51" s="241"/>
+      <c r="H51" s="241"/>
+      <c r="I51" s="241"/>
+      <c r="J51" s="241"/>
+      <c r="K51" s="241"/>
+      <c r="L51" s="242"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="246" t="s">
+        <v>449</v>
+      </c>
+      <c r="B52" s="241"/>
+      <c r="C52" s="241"/>
+      <c r="D52" s="241"/>
+      <c r="E52" s="241"/>
+      <c r="F52" s="241"/>
+      <c r="G52" s="241"/>
+      <c r="H52" s="241"/>
+      <c r="I52" s="241"/>
+      <c r="J52" s="241"/>
+      <c r="K52" s="241"/>
+      <c r="L52" s="242"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="240"/>
+      <c r="B53" s="241"/>
+      <c r="C53" s="241"/>
+      <c r="D53" s="241"/>
+      <c r="E53" s="241"/>
+      <c r="F53" s="241"/>
+      <c r="G53" s="241"/>
+      <c r="H53" s="241"/>
+      <c r="I53" s="241"/>
+      <c r="J53" s="241"/>
+      <c r="K53" s="241"/>
+      <c r="L53" s="242"/>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="240"/>
+      <c r="B54" s="241"/>
+      <c r="C54" s="241"/>
+      <c r="D54" s="241"/>
+      <c r="E54" s="241"/>
+      <c r="F54" s="241"/>
+      <c r="G54" s="241"/>
+      <c r="H54" s="241"/>
+      <c r="I54" s="241"/>
+      <c r="J54" s="241"/>
+      <c r="K54" s="241"/>
+      <c r="L54" s="242"/>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="240"/>
+      <c r="B55" s="241"/>
+      <c r="C55" s="241"/>
+      <c r="D55" s="241"/>
+      <c r="E55" s="241"/>
+      <c r="F55" s="241"/>
+      <c r="G55" s="241"/>
+      <c r="H55" s="241"/>
+      <c r="I55" s="241"/>
+      <c r="J55" s="241"/>
+      <c r="K55" s="241"/>
+      <c r="L55" s="242"/>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="240"/>
+      <c r="B56" s="241"/>
+      <c r="C56" s="241"/>
+      <c r="D56" s="241"/>
+      <c r="E56" s="241"/>
+      <c r="F56" s="241"/>
+      <c r="G56" s="241"/>
+      <c r="H56" s="241"/>
+      <c r="I56" s="241"/>
+      <c r="J56" s="241"/>
+      <c r="K56" s="241"/>
+      <c r="L56" s="242"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="240"/>
+      <c r="B57" s="241"/>
+      <c r="C57" s="241"/>
+      <c r="D57" s="241"/>
+      <c r="E57" s="241"/>
+      <c r="F57" s="241"/>
+      <c r="G57" s="241"/>
+      <c r="H57" s="241"/>
+      <c r="I57" s="241"/>
+      <c r="J57" s="241"/>
+      <c r="K57" s="241"/>
+      <c r="L57" s="242"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="240"/>
+      <c r="B58" s="241"/>
+      <c r="C58" s="241"/>
+      <c r="D58" s="241"/>
+      <c r="E58" s="241"/>
+      <c r="F58" s="241"/>
+      <c r="G58" s="241"/>
+      <c r="H58" s="241"/>
+      <c r="I58" s="241"/>
+      <c r="J58" s="241"/>
+      <c r="K58" s="241"/>
+      <c r="L58" s="242"/>
+    </row>
+    <row r="59" spans="1:12" ht="6" customHeight="1">
+      <c r="A59" s="247"/>
+      <c r="B59" s="248"/>
+      <c r="C59" s="248"/>
+      <c r="D59" s="248"/>
+      <c r="E59" s="248"/>
+      <c r="F59" s="248"/>
+      <c r="G59" s="248"/>
+      <c r="H59" s="248"/>
+      <c r="I59" s="248"/>
+      <c r="J59" s="248"/>
+      <c r="K59" s="248"/>
+      <c r="L59" s="249"/>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A60" s="243" t="s">
+        <v>424</v>
+      </c>
+      <c r="B60" s="244"/>
+      <c r="C60" s="244"/>
+      <c r="D60" s="244"/>
+      <c r="E60" s="244"/>
+      <c r="F60" s="244"/>
+      <c r="G60" s="244"/>
+      <c r="H60" s="244"/>
+      <c r="I60" s="244"/>
+      <c r="J60" s="244"/>
+      <c r="K60" s="244"/>
+      <c r="L60" s="245"/>
+    </row>
+    <row r="61" spans="1:12" ht="42.75" customHeight="1">
+      <c r="A61" s="250" t="s">
+        <v>394</v>
+      </c>
+      <c r="B61" s="251"/>
+      <c r="C61" s="251"/>
+      <c r="D61" s="251"/>
+      <c r="E61" s="251"/>
+      <c r="F61" s="251"/>
+      <c r="G61" s="251"/>
+      <c r="H61" s="251"/>
+      <c r="I61" s="251"/>
+      <c r="J61" s="251"/>
+      <c r="K61" s="251"/>
+      <c r="L61" s="252"/>
+    </row>
+    <row r="62" spans="1:12" ht="26.25" customHeight="1">
+      <c r="A62" s="246" t="s">
+        <v>441</v>
+      </c>
+      <c r="B62" s="241"/>
+      <c r="C62" s="241"/>
+      <c r="D62" s="241"/>
+      <c r="E62" s="241"/>
+      <c r="F62" s="241"/>
+      <c r="G62" s="241"/>
+      <c r="H62" s="241"/>
+      <c r="I62" s="241"/>
+      <c r="J62" s="241"/>
+      <c r="K62" s="241"/>
+      <c r="L62" s="242"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="246" t="s">
+        <v>435</v>
+      </c>
+      <c r="B63" s="241"/>
+      <c r="C63" s="241"/>
+      <c r="D63" s="241"/>
+      <c r="E63" s="241"/>
+      <c r="F63" s="241"/>
+      <c r="G63" s="241"/>
+      <c r="H63" s="241"/>
+      <c r="I63" s="241"/>
+      <c r="J63" s="241"/>
+      <c r="K63" s="241"/>
+      <c r="L63" s="242"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="246" t="s">
+        <v>442</v>
+      </c>
+      <c r="B64" s="241"/>
+      <c r="C64" s="241"/>
+      <c r="D64" s="241"/>
+      <c r="E64" s="241"/>
+      <c r="F64" s="241"/>
+      <c r="G64" s="241"/>
+      <c r="H64" s="241"/>
+      <c r="I64" s="241"/>
+      <c r="J64" s="241"/>
+      <c r="K64" s="241"/>
+      <c r="L64" s="242"/>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="246" t="s">
+        <v>436</v>
+      </c>
+      <c r="B65" s="241"/>
+      <c r="C65" s="241"/>
+      <c r="D65" s="241"/>
+      <c r="E65" s="241"/>
+      <c r="F65" s="241"/>
+      <c r="G65" s="241"/>
+      <c r="H65" s="241"/>
+      <c r="I65" s="241"/>
+      <c r="J65" s="241"/>
+      <c r="K65" s="241"/>
+      <c r="L65" s="242"/>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="246" t="s">
+        <v>437</v>
+      </c>
+      <c r="B66" s="241"/>
+      <c r="C66" s="241"/>
+      <c r="D66" s="241"/>
+      <c r="E66" s="241"/>
+      <c r="F66" s="241"/>
+      <c r="G66" s="241"/>
+      <c r="H66" s="241"/>
+      <c r="I66" s="241"/>
+      <c r="J66" s="241"/>
+      <c r="K66" s="241"/>
+      <c r="L66" s="242"/>
+    </row>
+    <row r="67" spans="1:12" ht="26.25" customHeight="1">
+      <c r="A67" s="246" t="s">
+        <v>443</v>
+      </c>
+      <c r="B67" s="241"/>
+      <c r="C67" s="241"/>
+      <c r="D67" s="241"/>
+      <c r="E67" s="241"/>
+      <c r="F67" s="241"/>
+      <c r="G67" s="241"/>
+      <c r="H67" s="241"/>
+      <c r="I67" s="241"/>
+      <c r="J67" s="241"/>
+      <c r="K67" s="241"/>
+      <c r="L67" s="242"/>
+    </row>
+    <row r="68" spans="1:12" ht="39.75" customHeight="1">
+      <c r="A68" s="246" t="s">
+        <v>444</v>
+      </c>
+      <c r="B68" s="351"/>
+      <c r="C68" s="351"/>
+      <c r="D68" s="351"/>
+      <c r="E68" s="351"/>
+      <c r="F68" s="351"/>
+      <c r="G68" s="351"/>
+      <c r="H68" s="351"/>
+      <c r="I68" s="351"/>
+      <c r="J68" s="351"/>
+      <c r="K68" s="351"/>
+      <c r="L68" s="352"/>
+    </row>
+    <row r="69" spans="1:12" ht="49.5" customHeight="1">
+      <c r="A69" s="246" t="s">
+        <v>445</v>
+      </c>
+      <c r="B69" s="241"/>
+      <c r="C69" s="241"/>
+      <c r="D69" s="241"/>
+      <c r="E69" s="241"/>
+      <c r="F69" s="241"/>
+      <c r="G69" s="241"/>
+      <c r="H69" s="241"/>
+      <c r="I69" s="241"/>
+      <c r="J69" s="241"/>
+      <c r="K69" s="241"/>
+      <c r="L69" s="242"/>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="246" t="s">
+        <v>440</v>
+      </c>
+      <c r="B70" s="241"/>
+      <c r="C70" s="241"/>
+      <c r="D70" s="241"/>
+      <c r="E70" s="241"/>
+      <c r="F70" s="241"/>
+      <c r="G70" s="241"/>
+      <c r="H70" s="241"/>
+      <c r="I70" s="241"/>
+      <c r="J70" s="241"/>
+      <c r="K70" s="241"/>
+      <c r="L70" s="242"/>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="246" t="s">
         <v>438</v>
       </c>
-      <c r="B44" s="242"/>
-      <c r="C44" s="242"/>
-      <c r="D44" s="242"/>
-      <c r="E44" s="242"/>
-      <c r="F44" s="242"/>
-      <c r="G44" s="242"/>
-      <c r="H44" s="242"/>
-      <c r="I44" s="242"/>
-      <c r="J44" s="242"/>
-      <c r="K44" s="242"/>
-      <c r="L44" s="243"/>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="241"/>
-      <c r="B45" s="242"/>
-      <c r="C45" s="242"/>
-      <c r="D45" s="242"/>
-      <c r="E45" s="242"/>
-      <c r="F45" s="242"/>
-      <c r="G45" s="242"/>
-      <c r="H45" s="242"/>
-      <c r="I45" s="242"/>
-      <c r="J45" s="242"/>
-      <c r="K45" s="242"/>
-      <c r="L45" s="243"/>
-    </row>
-    <row r="46" spans="1:12" ht="6" customHeight="1">
-      <c r="A46" s="245"/>
-      <c r="B46" s="246"/>
-      <c r="C46" s="246"/>
-      <c r="D46" s="246"/>
-      <c r="E46" s="246"/>
-      <c r="F46" s="246"/>
-      <c r="G46" s="246"/>
-      <c r="H46" s="246"/>
-      <c r="I46" s="246"/>
-      <c r="J46" s="246"/>
-      <c r="K46" s="246"/>
-      <c r="L46" s="247"/>
-    </row>
-    <row r="47" spans="1:12" ht="15.75">
-      <c r="A47" s="248" t="s">
-        <v>422</v>
-      </c>
-      <c r="B47" s="249"/>
-      <c r="C47" s="249"/>
-      <c r="D47" s="249"/>
-      <c r="E47" s="249"/>
-      <c r="F47" s="249"/>
-      <c r="G47" s="249"/>
-      <c r="H47" s="249"/>
-      <c r="I47" s="249"/>
-      <c r="J47" s="249"/>
-      <c r="K47" s="249"/>
-      <c r="L47" s="250"/>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="244" t="s">
-        <v>435</v>
-      </c>
-      <c r="B48" s="242"/>
-      <c r="C48" s="242"/>
-      <c r="D48" s="242"/>
-      <c r="E48" s="242"/>
-      <c r="F48" s="242"/>
-      <c r="G48" s="242"/>
-      <c r="H48" s="242"/>
-      <c r="I48" s="242"/>
-      <c r="J48" s="242"/>
-      <c r="K48" s="242"/>
-      <c r="L48" s="243"/>
-    </row>
-    <row r="49" spans="1:12" ht="6" customHeight="1">
-      <c r="A49" s="245"/>
-      <c r="B49" s="246"/>
-      <c r="C49" s="246"/>
-      <c r="D49" s="246"/>
-      <c r="E49" s="246"/>
-      <c r="F49" s="246"/>
-      <c r="G49" s="246"/>
-      <c r="H49" s="246"/>
-      <c r="I49" s="246"/>
-      <c r="J49" s="246"/>
-      <c r="K49" s="246"/>
-      <c r="L49" s="247"/>
-    </row>
-    <row r="50" spans="1:12" ht="15.75">
-      <c r="A50" s="248" t="s">
-        <v>423</v>
-      </c>
-      <c r="B50" s="249"/>
-      <c r="C50" s="249"/>
-      <c r="D50" s="249"/>
-      <c r="E50" s="249"/>
-      <c r="F50" s="249"/>
-      <c r="G50" s="249"/>
-      <c r="H50" s="249"/>
-      <c r="I50" s="249"/>
-      <c r="J50" s="249"/>
-      <c r="K50" s="249"/>
-      <c r="L50" s="250"/>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="244" t="s">
-        <v>430</v>
-      </c>
-      <c r="B51" s="242"/>
-      <c r="C51" s="242"/>
-      <c r="D51" s="242"/>
-      <c r="E51" s="242"/>
-      <c r="F51" s="242"/>
-      <c r="G51" s="242"/>
-      <c r="H51" s="242"/>
-      <c r="I51" s="242"/>
-      <c r="J51" s="242"/>
-      <c r="K51" s="242"/>
-      <c r="L51" s="243"/>
-    </row>
-    <row r="52" spans="1:12">
-      <c r="A52" s="244" t="s">
-        <v>436</v>
-      </c>
-      <c r="B52" s="242"/>
-      <c r="C52" s="242"/>
-      <c r="D52" s="242"/>
-      <c r="E52" s="242"/>
-      <c r="F52" s="242"/>
-      <c r="G52" s="242"/>
-      <c r="H52" s="242"/>
-      <c r="I52" s="242"/>
-      <c r="J52" s="242"/>
-      <c r="K52" s="242"/>
-      <c r="L52" s="243"/>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="A53" s="241"/>
-      <c r="B53" s="242"/>
-      <c r="C53" s="242"/>
-      <c r="D53" s="242"/>
-      <c r="E53" s="242"/>
-      <c r="F53" s="242"/>
-      <c r="G53" s="242"/>
-      <c r="H53" s="242"/>
-      <c r="I53" s="242"/>
-      <c r="J53" s="242"/>
-      <c r="K53" s="242"/>
-      <c r="L53" s="243"/>
-    </row>
-    <row r="54" spans="1:12">
-      <c r="A54" s="241"/>
-      <c r="B54" s="242"/>
-      <c r="C54" s="242"/>
-      <c r="D54" s="242"/>
-      <c r="E54" s="242"/>
-      <c r="F54" s="242"/>
-      <c r="G54" s="242"/>
-      <c r="H54" s="242"/>
-      <c r="I54" s="242"/>
-      <c r="J54" s="242"/>
-      <c r="K54" s="242"/>
-      <c r="L54" s="243"/>
-    </row>
-    <row r="55" spans="1:12">
-      <c r="A55" s="241"/>
-      <c r="B55" s="242"/>
-      <c r="C55" s="242"/>
-      <c r="D55" s="242"/>
-      <c r="E55" s="242"/>
-      <c r="F55" s="242"/>
-      <c r="G55" s="242"/>
-      <c r="H55" s="242"/>
-      <c r="I55" s="242"/>
-      <c r="J55" s="242"/>
-      <c r="K55" s="242"/>
-      <c r="L55" s="243"/>
-    </row>
-    <row r="56" spans="1:12">
-      <c r="A56" s="241"/>
-      <c r="B56" s="242"/>
-      <c r="C56" s="242"/>
-      <c r="D56" s="242"/>
-      <c r="E56" s="242"/>
-      <c r="F56" s="242"/>
-      <c r="G56" s="242"/>
-      <c r="H56" s="242"/>
-      <c r="I56" s="242"/>
-      <c r="J56" s="242"/>
-      <c r="K56" s="242"/>
-      <c r="L56" s="243"/>
-    </row>
-    <row r="57" spans="1:12">
-      <c r="A57" s="241"/>
-      <c r="B57" s="242"/>
-      <c r="C57" s="242"/>
-      <c r="D57" s="242"/>
-      <c r="E57" s="242"/>
-      <c r="F57" s="242"/>
-      <c r="G57" s="242"/>
-      <c r="H57" s="242"/>
-      <c r="I57" s="242"/>
-      <c r="J57" s="242"/>
-      <c r="K57" s="242"/>
-      <c r="L57" s="243"/>
-    </row>
-    <row r="58" spans="1:12">
-      <c r="A58" s="241"/>
-      <c r="B58" s="242"/>
-      <c r="C58" s="242"/>
-      <c r="D58" s="242"/>
-      <c r="E58" s="242"/>
-      <c r="F58" s="242"/>
-      <c r="G58" s="242"/>
-      <c r="H58" s="242"/>
-      <c r="I58" s="242"/>
-      <c r="J58" s="242"/>
-      <c r="K58" s="242"/>
-      <c r="L58" s="243"/>
-    </row>
-    <row r="59" spans="1:12">
-      <c r="A59" s="241"/>
-      <c r="B59" s="242"/>
-      <c r="C59" s="242"/>
-      <c r="D59" s="242"/>
-      <c r="E59" s="242"/>
-      <c r="F59" s="242"/>
-      <c r="G59" s="242"/>
-      <c r="H59" s="242"/>
-      <c r="I59" s="242"/>
-      <c r="J59" s="242"/>
-      <c r="K59" s="242"/>
-      <c r="L59" s="243"/>
-    </row>
-    <row r="60" spans="1:12" ht="6" customHeight="1">
-      <c r="A60" s="245"/>
-      <c r="B60" s="246"/>
-      <c r="C60" s="246"/>
-      <c r="D60" s="246"/>
-      <c r="E60" s="246"/>
-      <c r="F60" s="246"/>
-      <c r="G60" s="246"/>
-      <c r="H60" s="246"/>
-      <c r="I60" s="246"/>
-      <c r="J60" s="246"/>
-      <c r="K60" s="246"/>
-      <c r="L60" s="247"/>
-    </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A61" s="248" t="s">
-        <v>424</v>
-      </c>
-      <c r="B61" s="249"/>
-      <c r="C61" s="249"/>
-      <c r="D61" s="249"/>
-      <c r="E61" s="249"/>
-      <c r="F61" s="249"/>
-      <c r="G61" s="249"/>
-      <c r="H61" s="249"/>
-      <c r="I61" s="249"/>
-      <c r="J61" s="249"/>
-      <c r="K61" s="249"/>
-      <c r="L61" s="250"/>
-    </row>
-    <row r="62" spans="1:12" ht="42.75" customHeight="1">
-      <c r="A62" s="258" t="s">
-        <v>394</v>
-      </c>
-      <c r="B62" s="259"/>
-      <c r="C62" s="259"/>
-      <c r="D62" s="259"/>
-      <c r="E62" s="259"/>
-      <c r="F62" s="259"/>
-      <c r="G62" s="259"/>
-      <c r="H62" s="259"/>
-      <c r="I62" s="259"/>
-      <c r="J62" s="259"/>
-      <c r="K62" s="259"/>
-      <c r="L62" s="260"/>
-    </row>
-    <row r="63" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A63" s="244" t="s">
-        <v>442</v>
-      </c>
-      <c r="B63" s="242"/>
-      <c r="C63" s="242"/>
-      <c r="D63" s="242"/>
-      <c r="E63" s="242"/>
-      <c r="F63" s="242"/>
-      <c r="G63" s="242"/>
-      <c r="H63" s="242"/>
-      <c r="I63" s="242"/>
-      <c r="J63" s="242"/>
-      <c r="K63" s="242"/>
-      <c r="L63" s="243"/>
-    </row>
-    <row r="64" spans="1:12">
-      <c r="A64" s="244" t="s">
+      <c r="B71" s="241"/>
+      <c r="C71" s="241"/>
+      <c r="D71" s="241"/>
+      <c r="E71" s="241"/>
+      <c r="F71" s="241"/>
+      <c r="G71" s="241"/>
+      <c r="H71" s="241"/>
+      <c r="I71" s="241"/>
+      <c r="J71" s="241"/>
+      <c r="K71" s="241"/>
+      <c r="L71" s="242"/>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="246" t="s">
         <v>439</v>
       </c>
-      <c r="B64" s="242"/>
-      <c r="C64" s="242"/>
-      <c r="D64" s="242"/>
-      <c r="E64" s="242"/>
-      <c r="F64" s="242"/>
-      <c r="G64" s="242"/>
-      <c r="H64" s="242"/>
-      <c r="I64" s="242"/>
-      <c r="J64" s="242"/>
-      <c r="K64" s="242"/>
-      <c r="L64" s="243"/>
-    </row>
-    <row r="65" spans="1:12">
-      <c r="A65" s="244" t="s">
-        <v>440</v>
-      </c>
-      <c r="B65" s="242"/>
-      <c r="C65" s="242"/>
-      <c r="D65" s="242"/>
-      <c r="E65" s="242"/>
-      <c r="F65" s="242"/>
-      <c r="G65" s="242"/>
-      <c r="H65" s="242"/>
-      <c r="I65" s="242"/>
-      <c r="J65" s="242"/>
-      <c r="K65" s="242"/>
-      <c r="L65" s="243"/>
-    </row>
-    <row r="66" spans="1:12">
-      <c r="A66" s="244" t="s">
-        <v>441</v>
-      </c>
-      <c r="B66" s="242"/>
-      <c r="C66" s="242"/>
-      <c r="D66" s="242"/>
-      <c r="E66" s="242"/>
-      <c r="F66" s="242"/>
-      <c r="G66" s="242"/>
-      <c r="H66" s="242"/>
-      <c r="I66" s="242"/>
-      <c r="J66" s="242"/>
-      <c r="K66" s="242"/>
-      <c r="L66" s="243"/>
-    </row>
-    <row r="67" spans="1:12">
-      <c r="A67" s="244" t="s">
-        <v>444</v>
-      </c>
-      <c r="B67" s="242"/>
-      <c r="C67" s="242"/>
-      <c r="D67" s="242"/>
-      <c r="E67" s="242"/>
-      <c r="F67" s="242"/>
-      <c r="G67" s="242"/>
-      <c r="H67" s="242"/>
-      <c r="I67" s="242"/>
-      <c r="J67" s="242"/>
-      <c r="K67" s="242"/>
-      <c r="L67" s="243"/>
-    </row>
-    <row r="68" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A68" s="244" t="s">
-        <v>446</v>
-      </c>
-      <c r="B68" s="242"/>
-      <c r="C68" s="242"/>
-      <c r="D68" s="242"/>
-      <c r="E68" s="242"/>
-      <c r="F68" s="242"/>
-      <c r="G68" s="242"/>
-      <c r="H68" s="242"/>
-      <c r="I68" s="242"/>
-      <c r="J68" s="242"/>
-      <c r="K68" s="242"/>
-      <c r="L68" s="243"/>
-    </row>
-    <row r="69" spans="1:12" ht="39" customHeight="1">
-      <c r="A69" s="244" t="s">
-        <v>447</v>
-      </c>
-      <c r="B69" s="242"/>
-      <c r="C69" s="242"/>
-      <c r="D69" s="242"/>
-      <c r="E69" s="242"/>
-      <c r="F69" s="242"/>
-      <c r="G69" s="242"/>
-      <c r="H69" s="242"/>
-      <c r="I69" s="242"/>
-      <c r="J69" s="242"/>
-      <c r="K69" s="242"/>
-      <c r="L69" s="243"/>
-    </row>
-    <row r="70" spans="1:12">
-      <c r="A70" s="244" t="s">
-        <v>448</v>
-      </c>
-      <c r="B70" s="242"/>
-      <c r="C70" s="242"/>
-      <c r="D70" s="242"/>
-      <c r="E70" s="242"/>
-      <c r="F70" s="242"/>
-      <c r="G70" s="242"/>
-      <c r="H70" s="242"/>
-      <c r="I70" s="242"/>
-      <c r="J70" s="242"/>
-      <c r="K70" s="242"/>
-      <c r="L70" s="243"/>
-    </row>
-    <row r="71" spans="1:12">
-      <c r="A71" s="244" t="s">
-        <v>445</v>
-      </c>
-      <c r="B71" s="242"/>
-      <c r="C71" s="242"/>
-      <c r="D71" s="242"/>
-      <c r="E71" s="242"/>
-      <c r="F71" s="242"/>
-      <c r="G71" s="242"/>
-      <c r="H71" s="242"/>
-      <c r="I71" s="242"/>
-      <c r="J71" s="242"/>
-      <c r="K71" s="242"/>
-      <c r="L71" s="243"/>
-    </row>
-    <row r="72" spans="1:12">
-      <c r="A72" s="244" t="s">
-        <v>449</v>
-      </c>
-      <c r="B72" s="242"/>
-      <c r="C72" s="242"/>
-      <c r="D72" s="242"/>
-      <c r="E72" s="242"/>
-      <c r="F72" s="242"/>
-      <c r="G72" s="242"/>
-      <c r="H72" s="242"/>
-      <c r="I72" s="242"/>
-      <c r="J72" s="242"/>
-      <c r="K72" s="242"/>
-      <c r="L72" s="243"/>
+      <c r="B72" s="241"/>
+      <c r="C72" s="241"/>
+      <c r="D72" s="241"/>
+      <c r="E72" s="241"/>
+      <c r="F72" s="241"/>
+      <c r="G72" s="241"/>
+      <c r="H72" s="241"/>
+      <c r="I72" s="241"/>
+      <c r="J72" s="241"/>
+      <c r="K72" s="241"/>
+      <c r="L72" s="242"/>
     </row>
   </sheetData>
   <sheetProtection autoFilter="0"/>
   <mergeCells count="70">
-    <mergeCell ref="A56:L56"/>
-    <mergeCell ref="A57:L57"/>
-    <mergeCell ref="A58:L58"/>
-    <mergeCell ref="A42:L42"/>
-    <mergeCell ref="A52:L52"/>
-    <mergeCell ref="A53:L53"/>
-    <mergeCell ref="A54:L54"/>
-    <mergeCell ref="A55:L55"/>
-    <mergeCell ref="A43:L43"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="A45:L45"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A40:L40"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A46:L46"/>
+    <mergeCell ref="A49:L49"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A19:L19"/>
     <mergeCell ref="A48:L48"/>
-    <mergeCell ref="A51:L51"/>
-    <mergeCell ref="A46:L46"/>
+    <mergeCell ref="B22:K22"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="A37:L37"/>
+    <mergeCell ref="A38:L38"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A36:L36"/>
     <mergeCell ref="A69:L69"/>
     <mergeCell ref="A70:L70"/>
     <mergeCell ref="A71:L71"/>
     <mergeCell ref="A72:L72"/>
+    <mergeCell ref="A58:L58"/>
+    <mergeCell ref="A62:L62"/>
+    <mergeCell ref="A61:L61"/>
+    <mergeCell ref="A63:L63"/>
     <mergeCell ref="A59:L59"/>
-    <mergeCell ref="A63:L63"/>
-    <mergeCell ref="A62:L62"/>
+    <mergeCell ref="A66:L66"/>
+    <mergeCell ref="A67:L67"/>
+    <mergeCell ref="A65:L65"/>
+    <mergeCell ref="A60:L60"/>
     <mergeCell ref="A64:L64"/>
-    <mergeCell ref="A60:L60"/>
-    <mergeCell ref="A67:L67"/>
     <mergeCell ref="A68:L68"/>
-    <mergeCell ref="A66:L66"/>
-    <mergeCell ref="A61:L61"/>
-    <mergeCell ref="A65:L65"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A55:L55"/>
+    <mergeCell ref="A56:L56"/>
+    <mergeCell ref="A57:L57"/>
+    <mergeCell ref="A41:L41"/>
+    <mergeCell ref="A51:L51"/>
+    <mergeCell ref="A52:L52"/>
+    <mergeCell ref="A53:L53"/>
+    <mergeCell ref="A54:L54"/>
+    <mergeCell ref="A42:L42"/>
+    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="A44:L44"/>
     <mergeCell ref="A47:L47"/>
     <mergeCell ref="A50:L50"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A49:L49"/>
-    <mergeCell ref="B23:K23"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="A40:L40"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="A37:L37"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A41:L41"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A45:L45"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5696,7 +5734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5774,7 +5812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5912,7 +5950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5957,30 +5995,30 @@
       <c r="B2" s="147"/>
       <c r="C2" s="147"/>
       <c r="D2" s="148"/>
-      <c r="E2" s="270" t="s">
+      <c r="E2" s="272" t="s">
         <v>392</v>
       </c>
-      <c r="F2" s="270"/>
-      <c r="G2" s="270"/>
-      <c r="H2" s="270"/>
-      <c r="I2" s="270"/>
-      <c r="J2" s="270"/>
-      <c r="K2" s="270"/>
-      <c r="L2" s="270"/>
-      <c r="M2" s="270"/>
-      <c r="N2" s="270"/>
-      <c r="O2" s="270"/>
+      <c r="F2" s="272"/>
+      <c r="G2" s="272"/>
+      <c r="H2" s="272"/>
+      <c r="I2" s="272"/>
+      <c r="J2" s="272"/>
+      <c r="K2" s="272"/>
+      <c r="L2" s="272"/>
+      <c r="M2" s="272"/>
+      <c r="N2" s="272"/>
+      <c r="O2" s="272"/>
       <c r="P2" s="149" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="261" t="s">
+      <c r="Q2" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="262"/>
-      <c r="S2" s="262"/>
-      <c r="T2" s="262"/>
-      <c r="U2" s="262"/>
-      <c r="V2" s="263"/>
+      <c r="R2" s="264"/>
+      <c r="S2" s="264"/>
+      <c r="T2" s="264"/>
+      <c r="U2" s="264"/>
+      <c r="V2" s="265"/>
     </row>
     <row r="3" spans="1:34" ht="23.25" customHeight="1">
       <c r="A3" s="150" t="s">
@@ -5989,56 +6027,56 @@
       <c r="B3" s="151"/>
       <c r="C3" s="151"/>
       <c r="D3" s="152"/>
-      <c r="E3" s="271"/>
-      <c r="F3" s="271"/>
-      <c r="G3" s="271"/>
-      <c r="H3" s="271"/>
-      <c r="I3" s="271"/>
-      <c r="J3" s="271"/>
-      <c r="K3" s="271"/>
-      <c r="L3" s="271"/>
-      <c r="M3" s="271"/>
-      <c r="N3" s="271"/>
-      <c r="O3" s="271"/>
+      <c r="E3" s="273"/>
+      <c r="F3" s="273"/>
+      <c r="G3" s="273"/>
+      <c r="H3" s="273"/>
+      <c r="I3" s="273"/>
+      <c r="J3" s="273"/>
+      <c r="K3" s="273"/>
+      <c r="L3" s="273"/>
+      <c r="M3" s="273"/>
+      <c r="N3" s="273"/>
+      <c r="O3" s="273"/>
       <c r="P3" s="153" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="264" t="s">
+      <c r="Q3" s="266" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="265"/>
-      <c r="S3" s="265"/>
-      <c r="T3" s="265"/>
-      <c r="U3" s="265"/>
-      <c r="V3" s="266"/>
+      <c r="R3" s="267"/>
+      <c r="S3" s="267"/>
+      <c r="T3" s="267"/>
+      <c r="U3" s="267"/>
+      <c r="V3" s="268"/>
     </row>
     <row r="4" spans="1:34" s="154" customFormat="1" ht="20.25">
-      <c r="A4" s="267" t="s">
+      <c r="A4" s="269" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="268"/>
-      <c r="C4" s="268"/>
-      <c r="D4" s="268"/>
-      <c r="E4" s="268"/>
-      <c r="F4" s="268"/>
-      <c r="G4" s="269"/>
-      <c r="H4" s="267" t="s">
+      <c r="B4" s="270"/>
+      <c r="C4" s="270"/>
+      <c r="D4" s="270"/>
+      <c r="E4" s="270"/>
+      <c r="F4" s="270"/>
+      <c r="G4" s="271"/>
+      <c r="H4" s="269" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="268"/>
-      <c r="J4" s="268"/>
-      <c r="K4" s="268"/>
-      <c r="L4" s="268"/>
-      <c r="M4" s="268"/>
-      <c r="N4" s="268"/>
-      <c r="O4" s="268"/>
-      <c r="P4" s="268"/>
-      <c r="Q4" s="268"/>
-      <c r="R4" s="268"/>
-      <c r="S4" s="268"/>
-      <c r="T4" s="268"/>
-      <c r="U4" s="268"/>
-      <c r="V4" s="269"/>
+      <c r="I4" s="270"/>
+      <c r="J4" s="270"/>
+      <c r="K4" s="270"/>
+      <c r="L4" s="270"/>
+      <c r="M4" s="270"/>
+      <c r="N4" s="270"/>
+      <c r="O4" s="270"/>
+      <c r="P4" s="270"/>
+      <c r="Q4" s="270"/>
+      <c r="R4" s="270"/>
+      <c r="S4" s="270"/>
+      <c r="T4" s="270"/>
+      <c r="U4" s="270"/>
+      <c r="V4" s="271"/>
     </row>
     <row r="5" spans="1:34" ht="12" customHeight="1">
       <c r="A5" s="155"/>
@@ -9585,7 +9623,7 @@
       <c r="AB181" s="123"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:V41"/>
+  <autoFilter ref="A6:V41" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="5">
     <mergeCell ref="Q2:V2"/>
     <mergeCell ref="Q3:V3"/>
@@ -9602,16 +9640,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B41" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>$AA$7:$AA$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E7:E41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E7:E41" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>$AD$8:$AD$104</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="F7:F41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="F7:F41" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>$AE$7:$AE$40</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="G7:G41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="G7:G41" xr:uid="{00000000-0002-0000-0300-000003000000}">
       <formula1>$AF$7:$AF$103</formula1>
     </dataValidation>
   </dataValidations>
@@ -9626,13 +9664,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000004000000}">
           <x14:formula1>
             <xm:f>Lebensphasen!$A$2:$A$12</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0300-000005000000}">
           <x14:formula1>
             <xm:f>'Aufgaben+Tätigkeiten'!$B$3:$B$22</xm:f>
           </x14:formula1>
@@ -9645,7 +9683,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -9799,12 +9837,12 @@
       <c r="N3" s="80"/>
       <c r="O3" s="80"/>
       <c r="P3" s="80"/>
-      <c r="R3" s="284" t="s">
+      <c r="R3" s="282" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="284"/>
-      <c r="T3" s="284"/>
-      <c r="U3" s="284"/>
+      <c r="S3" s="282"/>
+      <c r="T3" s="282"/>
+      <c r="U3" s="282"/>
       <c r="W3" s="112" t="s">
         <v>25</v>
       </c>
@@ -9824,13 +9862,13 @@
       <c r="B4" s="291"/>
       <c r="C4" s="292"/>
       <c r="D4" s="198"/>
-      <c r="E4" s="275" t="s">
+      <c r="E4" s="300" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="277"/>
+      <c r="F4" s="301"/>
+      <c r="G4" s="301"/>
+      <c r="H4" s="301"/>
+      <c r="I4" s="302"/>
       <c r="J4" s="98"/>
       <c r="R4" s="99" t="s">
         <v>30</v>
@@ -9859,21 +9897,21 @@
       <c r="AB4" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="AC4" s="285" t="s">
+      <c r="AC4" s="283" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="286"/>
+      <c r="AD4" s="284"/>
     </row>
     <row r="5" spans="1:79" s="69" customFormat="1" ht="18">
       <c r="A5" s="293"/>
       <c r="B5" s="294"/>
       <c r="C5" s="295"/>
       <c r="D5" s="199"/>
-      <c r="E5" s="278"/>
-      <c r="F5" s="279"/>
-      <c r="G5" s="279"/>
-      <c r="H5" s="279"/>
-      <c r="I5" s="280"/>
+      <c r="E5" s="303"/>
+      <c r="F5" s="304"/>
+      <c r="G5" s="304"/>
+      <c r="H5" s="304"/>
+      <c r="I5" s="305"/>
       <c r="J5" s="100"/>
       <c r="R5" s="101" t="s">
         <v>38</v>
@@ -9903,10 +9941,10 @@
       <c r="AB5" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="AC5" s="285" t="s">
+      <c r="AC5" s="283" t="s">
         <v>43</v>
       </c>
-      <c r="AD5" s="286"/>
+      <c r="AD5" s="284"/>
     </row>
     <row r="6" spans="1:79" ht="18">
       <c r="A6" s="296"/>
@@ -10051,10 +10089,10 @@
       <c r="A9" s="81">
         <v>4</v>
       </c>
-      <c r="B9" s="272" t="s">
+      <c r="B9" s="285" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="273"/>
+      <c r="C9" s="286"/>
       <c r="D9" s="209" t="s">
         <v>58</v>
       </c>
@@ -10104,10 +10142,10 @@
       <c r="A10" s="81">
         <v>3</v>
       </c>
-      <c r="B10" s="272" t="s">
+      <c r="B10" s="285" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="273"/>
+      <c r="C10" s="286"/>
       <c r="D10" s="209" t="s">
         <v>62</v>
       </c>
@@ -10143,10 +10181,10 @@
       <c r="A11" s="81">
         <v>2</v>
       </c>
-      <c r="B11" s="272" t="s">
+      <c r="B11" s="285" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="273"/>
+      <c r="C11" s="286"/>
       <c r="D11" s="209" t="s">
         <v>67</v>
       </c>
@@ -10162,12 +10200,12 @@
         <v>54</v>
       </c>
       <c r="J11" s="66"/>
-      <c r="R11" s="274" t="s">
+      <c r="R11" s="299" t="s">
         <v>68</v>
       </c>
-      <c r="S11" s="274"/>
-      <c r="T11" s="274"/>
-      <c r="U11" s="274"/>
+      <c r="S11" s="299"/>
+      <c r="T11" s="299"/>
+      <c r="U11" s="299"/>
       <c r="W11" s="120">
         <v>2</v>
       </c>
@@ -10186,10 +10224,10 @@
       <c r="A12" s="81">
         <v>1</v>
       </c>
-      <c r="B12" s="272" t="s">
+      <c r="B12" s="285" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="273"/>
+      <c r="C12" s="286"/>
       <c r="D12" s="212" t="s">
         <v>42</v>
       </c>
@@ -10203,10 +10241,10 @@
         <v>59</v>
       </c>
       <c r="J12" s="66"/>
-      <c r="R12" s="274"/>
-      <c r="S12" s="274"/>
-      <c r="T12" s="274"/>
-      <c r="U12" s="274"/>
+      <c r="R12" s="299"/>
+      <c r="S12" s="299"/>
+      <c r="T12" s="299"/>
+      <c r="U12" s="299"/>
       <c r="W12" s="120">
         <v>2</v>
       </c>
@@ -10225,8 +10263,8 @@
       <c r="A13" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="282"/>
-      <c r="C13" s="283"/>
+      <c r="B13" s="306"/>
+      <c r="C13" s="307"/>
       <c r="D13" s="208"/>
       <c r="E13" s="85"/>
       <c r="F13" s="85"/>
@@ -10234,10 +10272,10 @@
       <c r="H13" s="85"/>
       <c r="I13" s="86"/>
       <c r="J13" s="66"/>
-      <c r="R13" s="274"/>
-      <c r="S13" s="274"/>
-      <c r="T13" s="274"/>
-      <c r="U13" s="274"/>
+      <c r="R13" s="299"/>
+      <c r="S13" s="299"/>
+      <c r="T13" s="299"/>
+      <c r="U13" s="299"/>
       <c r="W13" s="120">
         <v>2</v>
       </c>
@@ -10265,10 +10303,10 @@
       <c r="H14" s="219"/>
       <c r="I14" s="219"/>
       <c r="J14" s="66"/>
-      <c r="R14" s="274"/>
-      <c r="S14" s="274"/>
-      <c r="T14" s="274"/>
-      <c r="U14" s="274"/>
+      <c r="R14" s="299"/>
+      <c r="S14" s="299"/>
+      <c r="T14" s="299"/>
+      <c r="U14" s="299"/>
       <c r="W14" s="120">
         <v>2</v>
       </c>
@@ -10308,10 +10346,10 @@
         <v>401</v>
       </c>
       <c r="J15" s="66"/>
-      <c r="R15" s="274"/>
-      <c r="S15" s="274"/>
-      <c r="T15" s="274"/>
-      <c r="U15" s="274"/>
+      <c r="R15" s="299"/>
+      <c r="S15" s="299"/>
+      <c r="T15" s="299"/>
+      <c r="U15" s="299"/>
       <c r="W15" s="120">
         <v>3</v>
       </c>
@@ -10330,10 +10368,10 @@
       <c r="A16" s="220">
         <v>5</v>
       </c>
-      <c r="B16" s="281" t="s">
+      <c r="B16" s="280" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="281"/>
+      <c r="C16" s="280"/>
       <c r="D16" s="104" t="s">
         <v>387</v>
       </c>
@@ -10377,10 +10415,10 @@
       <c r="A17" s="220">
         <v>4</v>
       </c>
-      <c r="B17" s="281" t="s">
+      <c r="B17" s="280" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="281"/>
+      <c r="C17" s="280"/>
       <c r="D17" s="104" t="s">
         <v>388</v>
       </c>
@@ -10422,10 +10460,10 @@
       <c r="A18" s="220">
         <v>3</v>
       </c>
-      <c r="B18" s="281" t="s">
+      <c r="B18" s="280" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="281"/>
+      <c r="C18" s="280"/>
       <c r="D18" s="216"/>
       <c r="E18" s="216"/>
       <c r="F18" s="216"/>
@@ -10457,18 +10495,18 @@
       <c r="A19" s="220">
         <v>2</v>
       </c>
-      <c r="B19" s="281" t="s">
+      <c r="B19" s="280" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="281"/>
-      <c r="D19" s="302" t="s">
+      <c r="C19" s="280"/>
+      <c r="D19" s="279" t="s">
         <v>402</v>
       </c>
-      <c r="E19" s="302"/>
-      <c r="F19" s="302"/>
-      <c r="G19" s="302"/>
-      <c r="H19" s="302"/>
-      <c r="I19" s="302"/>
+      <c r="E19" s="279"/>
+      <c r="F19" s="279"/>
+      <c r="G19" s="279"/>
+      <c r="H19" s="279"/>
+      <c r="I19" s="279"/>
       <c r="J19" s="66"/>
       <c r="R19" s="109" t="s">
         <v>79</v>
@@ -10494,16 +10532,16 @@
       <c r="A20" s="220">
         <v>1</v>
       </c>
-      <c r="B20" s="281" t="s">
+      <c r="B20" s="280" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="281"/>
-      <c r="D20" s="302"/>
-      <c r="E20" s="302"/>
-      <c r="F20" s="302"/>
-      <c r="G20" s="302"/>
-      <c r="H20" s="302"/>
-      <c r="I20" s="302"/>
+      <c r="C20" s="280"/>
+      <c r="D20" s="279"/>
+      <c r="E20" s="279"/>
+      <c r="F20" s="279"/>
+      <c r="G20" s="279"/>
+      <c r="H20" s="279"/>
+      <c r="I20" s="279"/>
       <c r="J20" s="66"/>
       <c r="R20" s="109" t="s">
         <v>81</v>
@@ -10529,12 +10567,12 @@
       <c r="A21" s="66"/>
       <c r="B21" s="66"/>
       <c r="C21" s="66"/>
-      <c r="D21" s="302"/>
-      <c r="E21" s="302"/>
-      <c r="F21" s="302"/>
-      <c r="G21" s="302"/>
-      <c r="H21" s="302"/>
-      <c r="I21" s="302"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="279"/>
+      <c r="F21" s="279"/>
+      <c r="G21" s="279"/>
+      <c r="H21" s="279"/>
+      <c r="I21" s="279"/>
       <c r="J21" s="66"/>
       <c r="W21" s="120">
         <v>4</v>
@@ -10556,12 +10594,12 @@
       </c>
       <c r="B22" s="225"/>
       <c r="C22" s="225"/>
-      <c r="D22" s="302"/>
-      <c r="E22" s="302"/>
-      <c r="F22" s="302"/>
-      <c r="G22" s="302"/>
-      <c r="H22" s="302"/>
-      <c r="I22" s="302"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
+      <c r="F22" s="279"/>
+      <c r="G22" s="279"/>
+      <c r="H22" s="279"/>
+      <c r="I22" s="279"/>
       <c r="J22" s="66"/>
       <c r="W22" s="120">
         <v>4</v>
@@ -10581,16 +10619,16 @@
       <c r="A23" s="223">
         <v>5</v>
       </c>
-      <c r="B23" s="301" t="s">
+      <c r="B23" s="278" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="301"/>
-      <c r="D23" s="302"/>
-      <c r="E23" s="302"/>
-      <c r="F23" s="302"/>
-      <c r="G23" s="302"/>
-      <c r="H23" s="302"/>
-      <c r="I23" s="302"/>
+      <c r="C23" s="278"/>
+      <c r="D23" s="279"/>
+      <c r="E23" s="279"/>
+      <c r="F23" s="279"/>
+      <c r="G23" s="279"/>
+      <c r="H23" s="279"/>
+      <c r="I23" s="279"/>
       <c r="J23" s="66"/>
       <c r="R23" s="109"/>
       <c r="S23" s="109"/>
@@ -10614,16 +10652,16 @@
       <c r="A24" s="223">
         <v>3</v>
       </c>
-      <c r="B24" s="301" t="s">
+      <c r="B24" s="278" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="301"/>
-      <c r="D24" s="302"/>
-      <c r="E24" s="302"/>
-      <c r="F24" s="302"/>
-      <c r="G24" s="302"/>
-      <c r="H24" s="302"/>
-      <c r="I24" s="302"/>
+      <c r="C24" s="278"/>
+      <c r="D24" s="279"/>
+      <c r="E24" s="279"/>
+      <c r="F24" s="279"/>
+      <c r="G24" s="279"/>
+      <c r="H24" s="279"/>
+      <c r="I24" s="279"/>
       <c r="J24" s="66"/>
       <c r="W24" s="120">
         <v>4</v>
@@ -10643,16 +10681,16 @@
       <c r="A25" s="223">
         <v>1</v>
       </c>
-      <c r="B25" s="301" t="s">
+      <c r="B25" s="278" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="301"/>
-      <c r="D25" s="302"/>
-      <c r="E25" s="302"/>
-      <c r="F25" s="302"/>
-      <c r="G25" s="302"/>
-      <c r="H25" s="302"/>
-      <c r="I25" s="302"/>
+      <c r="C25" s="278"/>
+      <c r="D25" s="279"/>
+      <c r="E25" s="279"/>
+      <c r="F25" s="279"/>
+      <c r="G25" s="279"/>
+      <c r="H25" s="279"/>
+      <c r="I25" s="279"/>
       <c r="J25" s="66"/>
       <c r="W25" s="120">
         <v>5</v>
@@ -10672,12 +10710,12 @@
       <c r="A26" s="233"/>
       <c r="B26" s="233"/>
       <c r="C26" s="233"/>
-      <c r="D26" s="302"/>
-      <c r="E26" s="302"/>
-      <c r="F26" s="302"/>
-      <c r="G26" s="302"/>
-      <c r="H26" s="302"/>
-      <c r="I26" s="302"/>
+      <c r="D26" s="279"/>
+      <c r="E26" s="279"/>
+      <c r="F26" s="279"/>
+      <c r="G26" s="279"/>
+      <c r="H26" s="279"/>
+      <c r="I26" s="279"/>
       <c r="J26" s="66"/>
       <c r="W26" s="120"/>
       <c r="X26" s="112"/>
@@ -10688,12 +10726,12 @@
       <c r="A27" s="233"/>
       <c r="B27" s="233"/>
       <c r="C27" s="233"/>
-      <c r="D27" s="302"/>
-      <c r="E27" s="302"/>
-      <c r="F27" s="302"/>
-      <c r="G27" s="302"/>
-      <c r="H27" s="302"/>
-      <c r="I27" s="302"/>
+      <c r="D27" s="279"/>
+      <c r="E27" s="279"/>
+      <c r="F27" s="279"/>
+      <c r="G27" s="279"/>
+      <c r="H27" s="279"/>
+      <c r="I27" s="279"/>
       <c r="J27" s="66"/>
       <c r="W27" s="120"/>
       <c r="X27" s="112"/>
@@ -10704,12 +10742,12 @@
       <c r="A28" s="233"/>
       <c r="B28" s="233"/>
       <c r="C28" s="233"/>
-      <c r="D28" s="302"/>
-      <c r="E28" s="302"/>
-      <c r="F28" s="302"/>
-      <c r="G28" s="302"/>
-      <c r="H28" s="302"/>
-      <c r="I28" s="302"/>
+      <c r="D28" s="279"/>
+      <c r="E28" s="279"/>
+      <c r="F28" s="279"/>
+      <c r="G28" s="279"/>
+      <c r="H28" s="279"/>
+      <c r="I28" s="279"/>
       <c r="J28" s="66"/>
       <c r="W28" s="120"/>
       <c r="X28" s="112"/>
@@ -10720,12 +10758,12 @@
       <c r="A29" s="233"/>
       <c r="B29" s="233"/>
       <c r="C29" s="233"/>
-      <c r="D29" s="303"/>
-      <c r="E29" s="303"/>
-      <c r="F29" s="303"/>
-      <c r="G29" s="303"/>
-      <c r="H29" s="303"/>
-      <c r="I29" s="303"/>
+      <c r="D29" s="281"/>
+      <c r="E29" s="281"/>
+      <c r="F29" s="281"/>
+      <c r="G29" s="281"/>
+      <c r="H29" s="281"/>
+      <c r="I29" s="281"/>
       <c r="J29" s="66"/>
       <c r="W29" s="120"/>
       <c r="X29" s="112"/>
@@ -10797,10 +10835,10 @@
     </row>
     <row r="32" spans="1:38" ht="15.75" customHeight="1">
       <c r="A32" s="90"/>
-      <c r="B32" s="305" t="s">
+      <c r="B32" s="276" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="305"/>
+      <c r="C32" s="276"/>
       <c r="D32" s="205" t="s">
         <v>85</v>
       </c>
@@ -10836,21 +10874,21 @@
       <c r="A33" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="299" t="s">
+      <c r="B33" s="275" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="299"/>
+      <c r="C33" s="275"/>
       <c r="D33" s="197" t="s">
         <v>381</v>
       </c>
-      <c r="E33" s="299"/>
-      <c r="F33" s="299"/>
-      <c r="G33" s="299"/>
-      <c r="H33" s="299"/>
-      <c r="I33" s="299"/>
-      <c r="J33" s="299"/>
-      <c r="K33" s="299"/>
-      <c r="L33" s="299"/>
+      <c r="E33" s="275"/>
+      <c r="F33" s="275"/>
+      <c r="G33" s="275"/>
+      <c r="H33" s="275"/>
+      <c r="I33" s="275"/>
+      <c r="J33" s="275"/>
+      <c r="K33" s="275"/>
+      <c r="L33" s="275"/>
       <c r="M33"/>
       <c r="N33"/>
       <c r="O33"/>
@@ -10873,55 +10911,55 @@
       <c r="A34" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="299" t="s">
+      <c r="B34" s="275" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="299"/>
+      <c r="C34" s="275"/>
       <c r="D34" s="197" t="s">
         <v>382</v>
       </c>
-      <c r="E34" s="299" t="s">
+      <c r="E34" s="275" t="s">
         <v>384</v>
       </c>
-      <c r="F34" s="299"/>
-      <c r="G34" s="299"/>
-      <c r="H34" s="299"/>
-      <c r="I34" s="299"/>
-      <c r="J34" s="299"/>
-      <c r="K34" s="299"/>
-      <c r="L34" s="299"/>
+      <c r="F34" s="275"/>
+      <c r="G34" s="275"/>
+      <c r="H34" s="275"/>
+      <c r="I34" s="275"/>
+      <c r="J34" s="275"/>
+      <c r="K34" s="275"/>
+      <c r="L34" s="275"/>
       <c r="M34"/>
       <c r="N34"/>
       <c r="O34"/>
       <c r="P34"/>
-      <c r="R34" s="304" t="s">
+      <c r="R34" s="274" t="s">
         <v>89</v>
       </c>
-      <c r="S34" s="304"/>
-      <c r="T34" s="304"/>
-      <c r="U34" s="304"/>
+      <c r="S34" s="274"/>
+      <c r="T34" s="274"/>
+      <c r="U34" s="274"/>
     </row>
     <row r="35" spans="1:47" ht="218.25" customHeight="1">
       <c r="A35" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="299" t="s">
+      <c r="B35" s="275" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="299"/>
+      <c r="C35" s="275"/>
       <c r="D35" s="197" t="s">
         <v>383</v>
       </c>
-      <c r="E35" s="299" t="s">
+      <c r="E35" s="275" t="s">
         <v>385</v>
       </c>
-      <c r="F35" s="299"/>
-      <c r="G35" s="299"/>
-      <c r="H35" s="299"/>
-      <c r="I35" s="299"/>
-      <c r="J35" s="299"/>
-      <c r="K35" s="299"/>
-      <c r="L35" s="299"/>
+      <c r="F35" s="275"/>
+      <c r="G35" s="275"/>
+      <c r="H35" s="275"/>
+      <c r="I35" s="275"/>
+      <c r="J35" s="275"/>
+      <c r="K35" s="275"/>
+      <c r="L35" s="275"/>
       <c r="M35"/>
       <c r="N35"/>
       <c r="O35"/>
@@ -10931,21 +10969,21 @@
       <c r="A36" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="299" t="s">
+      <c r="B36" s="275" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="300"/>
+      <c r="C36" s="277"/>
       <c r="D36" s="206" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="299"/>
-      <c r="F36" s="299"/>
-      <c r="G36" s="299"/>
-      <c r="H36" s="299"/>
-      <c r="I36" s="299"/>
-      <c r="J36" s="299"/>
-      <c r="K36" s="299"/>
-      <c r="L36" s="299"/>
+      <c r="E36" s="275"/>
+      <c r="F36" s="275"/>
+      <c r="G36" s="275"/>
+      <c r="H36" s="275"/>
+      <c r="I36" s="275"/>
+      <c r="J36" s="275"/>
+      <c r="K36" s="275"/>
+      <c r="L36" s="275"/>
       <c r="M36"/>
       <c r="N36"/>
       <c r="O36"/>
@@ -12765,11 +12803,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="R34:U34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:L35"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="R11:U15"/>
+    <mergeCell ref="E4:I5"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A4:C6"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="E36:L36"/>
     <mergeCell ref="E33:L33"/>
@@ -12781,23 +12831,11 @@
     <mergeCell ref="D19:I28"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D29:I29"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A4:C6"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="R11:U15"/>
-    <mergeCell ref="E4:I5"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="R34:U34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:L35"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
   </mergeCells>
   <phoneticPr fontId="43" type="noConversion"/>
   <pageMargins left="0.196527777777778" right="0.196527777777778" top="0.39305555555555599" bottom="0.39305555555555599" header="0.51180555555555596" footer="0.196527777777778"/>
@@ -12812,7 +12850,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -12833,23 +12871,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25">
-      <c r="A1" s="306" t="s">
+      <c r="A1" s="308" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="306"/>
-      <c r="C1" s="306"/>
-      <c r="D1" s="306"/>
-      <c r="E1" s="306"/>
+      <c r="B1" s="308"/>
+      <c r="C1" s="308"/>
+      <c r="D1" s="308"/>
+      <c r="E1" s="308"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="307" t="s">
+      <c r="A2" s="309" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="307"/>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="307"/>
+      <c r="B2" s="309"/>
+      <c r="C2" s="309"/>
+      <c r="D2" s="309"/>
+      <c r="E2" s="309"/>
       <c r="F2" s="32"/>
       <c r="G2" s="32"/>
     </row>
@@ -12880,11 +12918,11 @@
       <c r="B6" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="308" t="s">
+      <c r="C6" s="310" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="309"/>
-      <c r="E6" s="309"/>
+      <c r="D6" s="311"/>
+      <c r="E6" s="311"/>
       <c r="G6" s="31"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
@@ -12896,11 +12934,11 @@
       <c r="G7" s="31"/>
     </row>
     <row r="8" spans="1:7" ht="14.25" customHeight="1">
-      <c r="C8" s="310" t="s">
+      <c r="C8" s="312" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="310"/>
-      <c r="E8" s="310"/>
+      <c r="D8" s="312"/>
+      <c r="E8" s="312"/>
       <c r="F8" s="55"/>
       <c r="G8" s="31"/>
     </row>
@@ -14056,7 +14094,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14070,29 +14108,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25">
-      <c r="A1" s="306" t="s">
+      <c r="A1" s="308" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="306"/>
-      <c r="C1" s="306"/>
-      <c r="D1" s="306"/>
-      <c r="E1" s="306"/>
+      <c r="B1" s="308"/>
+      <c r="C1" s="308"/>
+      <c r="D1" s="308"/>
+      <c r="E1" s="308"/>
     </row>
     <row r="2" spans="1:6" ht="14.25">
-      <c r="A2" s="307" t="s">
+      <c r="A2" s="309" t="s">
         <v>296</v>
       </c>
-      <c r="B2" s="307"/>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="307"/>
+      <c r="B2" s="309"/>
+      <c r="C2" s="309"/>
+      <c r="D2" s="309"/>
+      <c r="E2" s="309"/>
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" ht="14.25">
       <c r="C3" s="32"/>
-      <c r="D3" s="308"/>
-      <c r="E3" s="309"/>
-      <c r="F3" s="309"/>
+      <c r="D3" s="310"/>
+      <c r="E3" s="311"/>
+      <c r="F3" s="311"/>
     </row>
     <row r="4" spans="1:6" ht="14.25">
       <c r="A4" s="34" t="s">
@@ -14102,9 +14140,9 @@
         <v>96</v>
       </c>
       <c r="C4" s="35"/>
-      <c r="D4" s="310"/>
-      <c r="E4" s="323"/>
-      <c r="F4" s="323"/>
+      <c r="D4" s="312"/>
+      <c r="E4" s="313"/>
+      <c r="F4" s="313"/>
     </row>
     <row r="5" spans="1:6" ht="14.25">
       <c r="A5" s="38" t="s">
@@ -14135,7 +14173,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="324" t="s">
+      <c r="A9" s="314" t="s">
         <v>299</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -14143,13 +14181,13 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="325"/>
+      <c r="A10" s="315"/>
       <c r="B10" s="2" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="311" t="s">
+      <c r="A11" s="316" t="s">
         <v>302</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -14157,7 +14195,7 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="313"/>
+      <c r="A12" s="318"/>
       <c r="B12" s="2" t="s">
         <v>304</v>
       </c>
@@ -14187,7 +14225,7 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="314" t="s">
+      <c r="A16" s="319" t="s">
         <v>311</v>
       </c>
       <c r="B16" s="45" t="s">
@@ -14195,19 +14233,19 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="315"/>
+      <c r="A17" s="320"/>
       <c r="B17" s="1" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="316"/>
+      <c r="A18" s="321"/>
       <c r="B18" s="2" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="314" t="s">
+      <c r="A19" s="319" t="s">
         <v>315</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -14215,37 +14253,37 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="315"/>
+      <c r="A20" s="320"/>
       <c r="B20" s="1" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="315"/>
+      <c r="A21" s="320"/>
       <c r="B21" s="1" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="315"/>
+      <c r="A22" s="320"/>
       <c r="B22" s="46" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="315"/>
+      <c r="A23" s="320"/>
       <c r="B23" s="1" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="316"/>
+      <c r="A24" s="321"/>
       <c r="B24" s="2" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="317" t="s">
+      <c r="A25" s="322" t="s">
         <v>322</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -14253,37 +14291,37 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="318"/>
+      <c r="A26" s="323"/>
       <c r="B26" s="1" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="318"/>
+      <c r="A27" s="323"/>
       <c r="B27" s="1" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="318"/>
+      <c r="A28" s="323"/>
       <c r="B28" s="1" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="318"/>
+      <c r="A29" s="323"/>
       <c r="B29" s="1" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="319"/>
+      <c r="A30" s="324"/>
       <c r="B30" s="2" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A31" s="320" t="s">
+      <c r="A31" s="325" t="s">
         <v>329</v>
       </c>
       <c r="B31" s="47" t="s">
@@ -14291,44 +14329,44 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="321"/>
+      <c r="A32" s="326"/>
       <c r="B32" s="48" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="321"/>
+      <c r="A33" s="326"/>
       <c r="B33" s="48" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="321"/>
+      <c r="A34" s="326"/>
       <c r="B34" s="48" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="321"/>
+      <c r="A35" s="326"/>
       <c r="B35" s="48" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="321"/>
+      <c r="A36" s="326"/>
       <c r="B36" s="48" t="s">
         <v>335</v>
       </c>
       <c r="E36" s="49"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="322"/>
+      <c r="A37" s="327"/>
       <c r="B37" s="5" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="311" t="s">
+      <c r="A38" s="316" t="s">
         <v>337</v>
       </c>
       <c r="B38" s="50" t="s">
@@ -14336,25 +14374,25 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="312"/>
+      <c r="A39" s="317"/>
       <c r="B39" s="51" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="312"/>
+      <c r="A40" s="317"/>
       <c r="B40" s="51" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="312"/>
+      <c r="A41" s="317"/>
       <c r="B41" s="51" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="313"/>
+      <c r="A42" s="318"/>
       <c r="B42" s="5" t="s">
         <v>342</v>
       </c>
@@ -14379,17 +14417,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="A9:A10"/>
     <mergeCell ref="A38:A42"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A19:A24"/>
     <mergeCell ref="A25:A30"/>
     <mergeCell ref="A31:A37"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -14397,7 +14435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -14445,19 +14483,19 @@
       <c r="L3" s="24"/>
     </row>
     <row r="4" spans="1:15" s="7" customFormat="1" ht="23.25">
-      <c r="A4" s="343" t="s">
+      <c r="A4" s="328" t="s">
         <v>343</v>
       </c>
-      <c r="B4" s="343"/>
-      <c r="C4" s="343"/>
-      <c r="D4" s="343"/>
-      <c r="E4" s="343"/>
-      <c r="F4" s="343"/>
-      <c r="G4" s="343"/>
-      <c r="H4" s="343"/>
-      <c r="I4" s="343"/>
-      <c r="J4" s="343"/>
-      <c r="K4" s="343"/>
+      <c r="B4" s="328"/>
+      <c r="C4" s="328"/>
+      <c r="D4" s="328"/>
+      <c r="E4" s="328"/>
+      <c r="F4" s="328"/>
+      <c r="G4" s="328"/>
+      <c r="H4" s="328"/>
+      <c r="I4" s="328"/>
+      <c r="J4" s="328"/>
+      <c r="K4" s="328"/>
       <c r="L4" s="24"/>
     </row>
     <row r="5" spans="1:15" s="7" customFormat="1" ht="12.75" customHeight="1">
@@ -14475,10 +14513,10 @@
       <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:15" s="8" customFormat="1" ht="141" customHeight="1">
-      <c r="A6" s="327" t="s">
+      <c r="A6" s="329" t="s">
         <v>344</v>
       </c>
-      <c r="B6" s="328"/>
+      <c r="B6" s="330"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13" t="s">
         <v>345</v>
@@ -14488,18 +14526,18 @@
         <v>346</v>
       </c>
       <c r="G6" s="14"/>
-      <c r="H6" s="344" t="s">
+      <c r="H6" s="331" t="s">
         <v>347</v>
       </c>
-      <c r="I6" s="345"/>
-      <c r="J6" s="346"/>
+      <c r="I6" s="332"/>
+      <c r="J6" s="333"/>
       <c r="K6" s="26"/>
-      <c r="L6" s="326" t="s">
+      <c r="L6" s="342" t="s">
         <v>348</v>
       </c>
-      <c r="M6" s="327"/>
-      <c r="N6" s="327"/>
-      <c r="O6" s="328"/>
+      <c r="M6" s="329"/>
+      <c r="N6" s="329"/>
+      <c r="O6" s="330"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="23.25">
       <c r="A7" s="11"/>
@@ -14519,25 +14557,25 @@
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="337" t="s">
+      <c r="D8" s="335" t="s">
         <v>349</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="G8" s="342" t="s">
+      <c r="G8" s="341" t="s">
         <v>351</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="341" t="s">
+      <c r="J8" s="334" t="s">
         <v>352</v>
       </c>
-      <c r="K8" s="336" t="s">
+      <c r="K8" s="338" t="s">
         <v>351</v>
       </c>
-      <c r="L8" s="341" t="s">
+      <c r="L8" s="334" t="s">
         <v>353</v>
       </c>
       <c r="N8" s="27" t="s">
@@ -14551,16 +14589,16 @@
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="338"/>
+      <c r="D9" s="336"/>
       <c r="E9" s="11"/>
       <c r="F9" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="G9" s="342"/>
+      <c r="G9" s="341"/>
       <c r="H9" s="19"/>
-      <c r="J9" s="341"/>
-      <c r="K9" s="336"/>
-      <c r="L9" s="341"/>
+      <c r="J9" s="334"/>
+      <c r="K9" s="338"/>
+      <c r="L9" s="334"/>
       <c r="N9" s="27" t="s">
         <v>16</v>
       </c>
@@ -14572,17 +14610,17 @@
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="11"/>
-      <c r="D10" s="338"/>
+      <c r="D10" s="336"/>
       <c r="E10" s="11"/>
       <c r="F10" s="17" t="s">
         <v>355</v>
       </c>
-      <c r="G10" s="342"/>
+      <c r="G10" s="341"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
-      <c r="J10" s="341"/>
-      <c r="K10" s="336"/>
-      <c r="L10" s="341"/>
+      <c r="J10" s="334"/>
+      <c r="K10" s="338"/>
+      <c r="L10" s="334"/>
       <c r="N10" s="27" t="s">
         <v>17</v>
       </c>
@@ -14594,15 +14632,15 @@
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="11"/>
-      <c r="D11" s="338"/>
+      <c r="D11" s="336"/>
       <c r="E11" s="11"/>
       <c r="F11" s="17"/>
-      <c r="G11" s="342"/>
+      <c r="G11" s="341"/>
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
-      <c r="J11" s="341"/>
-      <c r="K11" s="336"/>
-      <c r="L11" s="341"/>
+      <c r="J11" s="334"/>
+      <c r="K11" s="338"/>
+      <c r="L11" s="334"/>
       <c r="N11" s="27" t="s">
         <v>18</v>
       </c>
@@ -14618,15 +14656,15 @@
         <v>9</v>
       </c>
       <c r="C12" s="11"/>
-      <c r="D12" s="339"/>
+      <c r="D12" s="337"/>
       <c r="E12" s="11"/>
       <c r="F12" s="17"/>
-      <c r="G12" s="342"/>
+      <c r="G12" s="341"/>
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
-      <c r="J12" s="341"/>
-      <c r="K12" s="336"/>
-      <c r="L12" s="341"/>
+      <c r="J12" s="334"/>
+      <c r="K12" s="338"/>
+      <c r="L12" s="334"/>
       <c r="N12" s="27" t="s">
         <v>19</v>
       </c>
@@ -14662,27 +14700,27 @@
         <v>9</v>
       </c>
       <c r="C14" s="11"/>
-      <c r="D14" s="341" t="s">
+      <c r="D14" s="334" t="s">
         <v>345</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="340" t="s">
+      <c r="G14" s="350" t="s">
         <v>351</v>
       </c>
-      <c r="H14" s="337" t="s">
+      <c r="H14" s="335" t="s">
         <v>356</v>
       </c>
-      <c r="I14" s="348" t="s">
+      <c r="I14" s="340" t="s">
         <v>351</v>
       </c>
-      <c r="J14" s="335" t="s">
+      <c r="J14" s="349" t="s">
         <v>357</v>
       </c>
-      <c r="K14" s="336" t="s">
+      <c r="K14" s="338" t="s">
         <v>351</v>
       </c>
-      <c r="L14" s="335" t="s">
+      <c r="L14" s="349" t="s">
         <v>353</v>
       </c>
       <c r="N14" s="27" t="s">
@@ -14700,17 +14738,17 @@
         <v>9</v>
       </c>
       <c r="C15" s="11"/>
-      <c r="D15" s="341"/>
+      <c r="D15" s="334"/>
       <c r="E15" s="11"/>
       <c r="F15" s="17" t="s">
         <v>355</v>
       </c>
-      <c r="G15" s="340"/>
-      <c r="H15" s="338"/>
-      <c r="I15" s="348"/>
-      <c r="J15" s="335"/>
-      <c r="K15" s="336"/>
-      <c r="L15" s="335"/>
+      <c r="G15" s="350"/>
+      <c r="H15" s="336"/>
+      <c r="I15" s="340"/>
+      <c r="J15" s="349"/>
+      <c r="K15" s="338"/>
+      <c r="L15" s="349"/>
       <c r="N15" s="27" t="s">
         <v>16</v>
       </c>
@@ -14726,17 +14764,17 @@
         <v>9</v>
       </c>
       <c r="C16" s="11"/>
-      <c r="D16" s="341"/>
+      <c r="D16" s="334"/>
       <c r="E16" s="11"/>
       <c r="F16" s="17" t="s">
         <v>358</v>
       </c>
-      <c r="G16" s="340"/>
-      <c r="H16" s="338"/>
-      <c r="I16" s="348"/>
-      <c r="J16" s="335"/>
-      <c r="K16" s="336"/>
-      <c r="L16" s="335"/>
+      <c r="G16" s="350"/>
+      <c r="H16" s="336"/>
+      <c r="I16" s="340"/>
+      <c r="J16" s="349"/>
+      <c r="K16" s="338"/>
+      <c r="L16" s="349"/>
       <c r="N16" s="27" t="s">
         <v>17</v>
       </c>
@@ -14745,22 +14783,22 @@
       </c>
     </row>
     <row r="17" spans="1:15" s="7" customFormat="1" ht="21" customHeight="1">
-      <c r="A17" s="329" t="s">
+      <c r="A17" s="343" t="s">
         <v>359</v>
       </c>
-      <c r="B17" s="330"/>
+      <c r="B17" s="344"/>
       <c r="C17" s="11"/>
-      <c r="D17" s="341"/>
+      <c r="D17" s="334"/>
       <c r="E17" s="11"/>
       <c r="F17" s="17" t="s">
         <v>360</v>
       </c>
-      <c r="G17" s="340"/>
-      <c r="H17" s="338"/>
-      <c r="I17" s="348"/>
-      <c r="J17" s="335"/>
-      <c r="K17" s="336"/>
-      <c r="L17" s="335"/>
+      <c r="G17" s="350"/>
+      <c r="H17" s="336"/>
+      <c r="I17" s="340"/>
+      <c r="J17" s="349"/>
+      <c r="K17" s="338"/>
+      <c r="L17" s="349"/>
       <c r="N17" s="27" t="s">
         <v>18</v>
       </c>
@@ -14769,20 +14807,20 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="7" customFormat="1" ht="21" customHeight="1">
-      <c r="A18" s="331"/>
-      <c r="B18" s="332"/>
+      <c r="A18" s="345"/>
+      <c r="B18" s="346"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="341"/>
+      <c r="D18" s="334"/>
       <c r="E18" s="11"/>
       <c r="F18" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="G18" s="340"/>
-      <c r="H18" s="338"/>
-      <c r="I18" s="348"/>
-      <c r="J18" s="335"/>
-      <c r="K18" s="336"/>
-      <c r="L18" s="335"/>
+      <c r="G18" s="350"/>
+      <c r="H18" s="336"/>
+      <c r="I18" s="340"/>
+      <c r="J18" s="349"/>
+      <c r="K18" s="338"/>
+      <c r="L18" s="349"/>
       <c r="M18" s="18"/>
       <c r="N18" s="27" t="s">
         <v>19</v>
@@ -14792,42 +14830,42 @@
       </c>
     </row>
     <row r="19" spans="1:15" s="7" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="331"/>
-      <c r="B19" s="332"/>
+      <c r="A19" s="345"/>
+      <c r="B19" s="346"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="341"/>
+      <c r="D19" s="334"/>
       <c r="E19" s="11"/>
       <c r="F19" s="17" t="s">
         <v>362</v>
       </c>
-      <c r="G19" s="340"/>
-      <c r="H19" s="338"/>
+      <c r="G19" s="350"/>
+      <c r="H19" s="336"/>
       <c r="I19" s="18"/>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
     </row>
     <row r="20" spans="1:15" s="7" customFormat="1" ht="21" customHeight="1">
-      <c r="A20" s="331"/>
-      <c r="B20" s="332"/>
+      <c r="A20" s="345"/>
+      <c r="B20" s="346"/>
       <c r="C20" s="11"/>
-      <c r="D20" s="341"/>
+      <c r="D20" s="334"/>
       <c r="E20" s="11"/>
       <c r="F20" s="17" t="s">
         <v>363</v>
       </c>
-      <c r="G20" s="340"/>
-      <c r="H20" s="338"/>
-      <c r="I20" s="342" t="s">
+      <c r="G20" s="350"/>
+      <c r="H20" s="336"/>
+      <c r="I20" s="341" t="s">
         <v>351</v>
       </c>
-      <c r="J20" s="335" t="s">
+      <c r="J20" s="349" t="s">
         <v>364</v>
       </c>
-      <c r="K20" s="347" t="s">
+      <c r="K20" s="339" t="s">
         <v>351</v>
       </c>
-      <c r="L20" s="335" t="s">
+      <c r="L20" s="349" t="s">
         <v>365</v>
       </c>
       <c r="N20" s="27" t="s">
@@ -14838,20 +14876,20 @@
       </c>
     </row>
     <row r="21" spans="1:15" s="7" customFormat="1" ht="21" customHeight="1">
-      <c r="A21" s="333"/>
-      <c r="B21" s="334"/>
+      <c r="A21" s="347"/>
+      <c r="B21" s="348"/>
       <c r="C21" s="11"/>
-      <c r="D21" s="341"/>
+      <c r="D21" s="334"/>
       <c r="E21" s="11"/>
       <c r="F21" s="17" t="s">
         <v>367</v>
       </c>
-      <c r="G21" s="340"/>
-      <c r="H21" s="338"/>
-      <c r="I21" s="342"/>
-      <c r="J21" s="335"/>
-      <c r="K21" s="347"/>
-      <c r="L21" s="335"/>
+      <c r="G21" s="350"/>
+      <c r="H21" s="336"/>
+      <c r="I21" s="341"/>
+      <c r="J21" s="349"/>
+      <c r="K21" s="339"/>
+      <c r="L21" s="349"/>
       <c r="N21" s="27" t="s">
         <v>16</v>
       </c>
@@ -14863,17 +14901,17 @@
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="11"/>
-      <c r="D22" s="341"/>
+      <c r="D22" s="334"/>
       <c r="E22" s="11"/>
       <c r="F22" s="17" t="s">
         <v>368</v>
       </c>
-      <c r="G22" s="340"/>
-      <c r="H22" s="338"/>
-      <c r="I22" s="342"/>
-      <c r="J22" s="335"/>
-      <c r="K22" s="347"/>
-      <c r="L22" s="335"/>
+      <c r="G22" s="350"/>
+      <c r="H22" s="336"/>
+      <c r="I22" s="341"/>
+      <c r="J22" s="349"/>
+      <c r="K22" s="339"/>
+      <c r="L22" s="349"/>
       <c r="N22" s="27" t="s">
         <v>17</v>
       </c>
@@ -14885,17 +14923,17 @@
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="11"/>
-      <c r="D23" s="341"/>
+      <c r="D23" s="334"/>
       <c r="E23" s="11"/>
       <c r="F23" s="17" t="s">
         <v>369</v>
       </c>
-      <c r="G23" s="340"/>
-      <c r="H23" s="338"/>
-      <c r="I23" s="342"/>
-      <c r="J23" s="335"/>
-      <c r="K23" s="347"/>
-      <c r="L23" s="335"/>
+      <c r="G23" s="350"/>
+      <c r="H23" s="336"/>
+      <c r="I23" s="341"/>
+      <c r="J23" s="349"/>
+      <c r="K23" s="339"/>
+      <c r="L23" s="349"/>
       <c r="N23" s="27" t="s">
         <v>18</v>
       </c>
@@ -14907,15 +14945,15 @@
       <c r="A24" s="16"/>
       <c r="B24" s="16"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="341"/>
+      <c r="D24" s="334"/>
       <c r="E24" s="11"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="340"/>
-      <c r="H24" s="339"/>
-      <c r="I24" s="342"/>
-      <c r="J24" s="335"/>
-      <c r="K24" s="347"/>
-      <c r="L24" s="335"/>
+      <c r="G24" s="350"/>
+      <c r="H24" s="337"/>
+      <c r="I24" s="341"/>
+      <c r="J24" s="349"/>
+      <c r="K24" s="339"/>
+      <c r="L24" s="349"/>
       <c r="N24" s="27" t="s">
         <v>19</v>
       </c>
@@ -14944,16 +14982,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="D14:D24"/>
-    <mergeCell ref="H14:H24"/>
-    <mergeCell ref="K8:K12"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="J8:J12"/>
-    <mergeCell ref="I14:I18"/>
-    <mergeCell ref="I20:I24"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="A17:B21"/>
     <mergeCell ref="J14:J18"/>
@@ -14965,6 +14993,16 @@
     <mergeCell ref="L14:L18"/>
     <mergeCell ref="L20:L24"/>
     <mergeCell ref="G8:G12"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="D14:D24"/>
+    <mergeCell ref="H14:H24"/>
+    <mergeCell ref="K8:K12"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="J8:J12"/>
+    <mergeCell ref="I14:I18"/>
+    <mergeCell ref="I20:I24"/>
   </mergeCells>
   <phoneticPr fontId="43" type="noConversion"/>
   <pageMargins left="0.31388888888888899" right="0.31388888888888899" top="0.78680555555555598" bottom="0.39305555555555599" header="0.31388888888888899" footer="0.31388888888888899"/>

</xml_diff>